<commit_message>
fixed marksheet subject duplicate logic
</commit_message>
<xml_diff>
--- a/apps/backend/public/data/ccf-ba-subjects.xlsx
+++ b/apps/backend/public/data/ccf-ba-subjects.xlsx
@@ -47,10 +47,10 @@
     <t>Specialization</t>
   </si>
   <si>
-    <t>Subject Type</t>
-  </si>
-  <si>
-    <t>Subject Name</t>
+    <t>Subject Type as per Marksheet</t>
+  </si>
+  <si>
+    <t>Subject Code as per Marksheet</t>
   </si>
   <si>
     <t>Credit</t>
@@ -1020,7 +1020,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1029,6 +1029,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1597,16 +1600,18 @@
   <sheetPr/>
   <dimension ref="A1:Q86"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F84" sqref="F84"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8"/>
   <cols>
-    <col min="7" max="7" width="10.6796875" customWidth="1"/>
+    <col min="6" max="6" width="11.5859375" customWidth="1"/>
+    <col min="7" max="7" width="27.078125" customWidth="1"/>
+    <col min="8" max="8" width="24.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" ht="29" spans="1:17">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1625,10 +1630,10 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
@@ -1655,7 +1660,7 @@
       <c r="P1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="10" t="s">
+      <c r="Q1" s="11" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1674,10 +1679,10 @@
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="5" t="s">
         <v>21</v>
       </c>
       <c r="I2" s="2">
@@ -1696,7 +1701,7 @@
       <c r="P2" s="2">
         <v>100</v>
       </c>
-      <c r="Q2" s="9"/>
+      <c r="Q2" s="10"/>
     </row>
     <row r="3" ht="17.6" spans="1:17">
       <c r="A3" s="2" t="s">
@@ -1713,10 +1718,10 @@
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="H3" s="5" t="s">
         <v>22</v>
       </c>
       <c r="I3" s="2">
@@ -1735,7 +1740,7 @@
       <c r="P3" s="2">
         <v>100</v>
       </c>
-      <c r="Q3" s="9"/>
+      <c r="Q3" s="10"/>
     </row>
     <row r="4" ht="17.6" spans="1:17">
       <c r="A4" s="2" t="s">
@@ -1752,10 +1757,10 @@
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
-      <c r="G4" s="3" t="s">
+      <c r="G4" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="H4" s="5" t="s">
         <v>23</v>
       </c>
       <c r="I4" s="2">
@@ -1774,7 +1779,7 @@
       <c r="P4" s="2">
         <v>100</v>
       </c>
-      <c r="Q4" s="9"/>
+      <c r="Q4" s="10"/>
     </row>
     <row r="5" ht="17.6" spans="1:17">
       <c r="A5" s="2" t="s">
@@ -1791,10 +1796,10 @@
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
-      <c r="G5" s="3" t="s">
+      <c r="G5" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="H5" s="4" t="s">
+      <c r="H5" s="5" t="s">
         <v>24</v>
       </c>
       <c r="I5" s="2">
@@ -1813,7 +1818,7 @@
       <c r="P5" s="2">
         <v>100</v>
       </c>
-      <c r="Q5" s="9"/>
+      <c r="Q5" s="10"/>
     </row>
     <row r="6" ht="17.6" spans="1:17">
       <c r="A6" s="2" t="s">
@@ -1830,10 +1835,10 @@
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
-      <c r="G6" s="3" t="s">
+      <c r="G6" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="H6" s="4" t="s">
+      <c r="H6" s="5" t="s">
         <v>25</v>
       </c>
       <c r="I6" s="2">
@@ -1852,7 +1857,7 @@
       <c r="P6" s="2">
         <v>100</v>
       </c>
-      <c r="Q6" s="9"/>
+      <c r="Q6" s="10"/>
     </row>
     <row r="7" ht="17.6" spans="1:17">
       <c r="A7" s="2" t="s">
@@ -1869,10 +1874,10 @@
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
-      <c r="G7" s="3" t="s">
+      <c r="G7" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="H7" s="4" t="s">
+      <c r="H7" s="5" t="s">
         <v>27</v>
       </c>
       <c r="I7" s="2">
@@ -1889,7 +1894,7 @@
       <c r="P7" s="2">
         <v>100</v>
       </c>
-      <c r="Q7" s="9"/>
+      <c r="Q7" s="10"/>
     </row>
     <row r="8" ht="17.6" spans="1:17">
       <c r="A8" s="2" t="s">
@@ -1906,10 +1911,10 @@
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
-      <c r="G8" s="3" t="s">
+      <c r="G8" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="H8" s="4" t="s">
+      <c r="H8" s="5" t="s">
         <v>28</v>
       </c>
       <c r="I8" s="2">
@@ -1928,7 +1933,7 @@
       <c r="P8" s="2">
         <v>100</v>
       </c>
-      <c r="Q8" s="9"/>
+      <c r="Q8" s="10"/>
     </row>
     <row r="9" ht="17.6" spans="1:17">
       <c r="A9" s="2" t="s">
@@ -1945,10 +1950,10 @@
       </c>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
-      <c r="G9" s="3" t="s">
+      <c r="G9" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="H9" s="4" t="s">
+      <c r="H9" s="5" t="s">
         <v>29</v>
       </c>
       <c r="I9" s="2">
@@ -1965,7 +1970,7 @@
       <c r="P9" s="2">
         <v>100</v>
       </c>
-      <c r="Q9" s="9"/>
+      <c r="Q9" s="10"/>
     </row>
     <row r="10" ht="17.6" spans="1:17">
       <c r="A10" s="2" t="s">
@@ -1982,10 +1987,10 @@
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
-      <c r="G10" s="3" t="s">
+      <c r="G10" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="H10" s="4" t="s">
+      <c r="H10" s="5" t="s">
         <v>30</v>
       </c>
       <c r="I10" s="2">
@@ -2004,7 +2009,7 @@
       <c r="P10" s="2">
         <v>100</v>
       </c>
-      <c r="Q10" s="9"/>
+      <c r="Q10" s="10"/>
     </row>
     <row r="11" ht="17.6" spans="1:17">
       <c r="A11" s="2" t="s">
@@ -2021,10 +2026,10 @@
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
-      <c r="G11" s="3" t="s">
+      <c r="G11" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="H11" s="4" t="s">
+      <c r="H11" s="5" t="s">
         <v>31</v>
       </c>
       <c r="I11" s="2">
@@ -2043,7 +2048,7 @@
       <c r="P11" s="2">
         <v>100</v>
       </c>
-      <c r="Q11" s="9"/>
+      <c r="Q11" s="10"/>
     </row>
     <row r="12" ht="17.6" spans="1:17">
       <c r="A12" s="2" t="s">
@@ -2060,10 +2065,10 @@
       </c>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
-      <c r="G12" s="3" t="s">
+      <c r="G12" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="H12" s="4" t="s">
+      <c r="H12" s="5" t="s">
         <v>33</v>
       </c>
       <c r="I12" s="2">
@@ -2082,7 +2087,7 @@
       <c r="P12" s="2">
         <v>100</v>
       </c>
-      <c r="Q12" s="9"/>
+      <c r="Q12" s="10"/>
     </row>
     <row r="13" ht="17.6" spans="1:17">
       <c r="A13" s="2" t="s">
@@ -2099,10 +2104,10 @@
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
-      <c r="G13" s="3" t="s">
+      <c r="G13" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="H13" s="5" t="s">
+      <c r="H13" s="6" t="s">
         <v>34</v>
       </c>
       <c r="I13" s="2">
@@ -2121,7 +2126,7 @@
       <c r="P13" s="2">
         <v>100</v>
       </c>
-      <c r="Q13" s="9"/>
+      <c r="Q13" s="10"/>
     </row>
     <row r="14" ht="17.6" spans="1:17">
       <c r="A14" s="2" t="s">
@@ -2138,10 +2143,10 @@
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
-      <c r="G14" s="3" t="s">
+      <c r="G14" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="H14" s="5" t="s">
+      <c r="H14" s="6" t="s">
         <v>35</v>
       </c>
       <c r="I14" s="2">
@@ -2160,7 +2165,7 @@
       <c r="P14" s="2">
         <v>100</v>
       </c>
-      <c r="Q14" s="9"/>
+      <c r="Q14" s="10"/>
     </row>
     <row r="15" ht="17.6" spans="1:17">
       <c r="A15" s="2" t="s">
@@ -2177,10 +2182,10 @@
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
-      <c r="G15" s="3" t="s">
+      <c r="G15" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="H15" s="6" t="s">
+      <c r="H15" s="7" t="s">
         <v>36</v>
       </c>
       <c r="I15" s="2">
@@ -2199,7 +2204,7 @@
       <c r="P15" s="2">
         <v>100</v>
       </c>
-      <c r="Q15" s="9"/>
+      <c r="Q15" s="10"/>
     </row>
     <row r="16" ht="17.6" spans="1:17">
       <c r="A16" s="2" t="s">
@@ -2216,10 +2221,10 @@
       </c>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
-      <c r="G16" s="3" t="s">
+      <c r="G16" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="H16" s="5" t="s">
+      <c r="H16" s="6" t="s">
         <v>37</v>
       </c>
       <c r="I16" s="2">
@@ -2238,7 +2243,7 @@
       <c r="P16" s="2">
         <v>100</v>
       </c>
-      <c r="Q16" s="9"/>
+      <c r="Q16" s="10"/>
     </row>
     <row r="17" ht="17.6" spans="1:17">
       <c r="A17" s="2" t="s">
@@ -2255,10 +2260,10 @@
       </c>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
-      <c r="G17" s="3" t="s">
+      <c r="G17" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="H17" s="7" t="s">
+      <c r="H17" s="8" t="s">
         <v>38</v>
       </c>
       <c r="I17" s="2">
@@ -2277,7 +2282,7 @@
       <c r="P17" s="2">
         <v>100</v>
       </c>
-      <c r="Q17" s="9"/>
+      <c r="Q17" s="10"/>
     </row>
     <row r="18" ht="17.6" spans="1:17">
       <c r="A18" s="2" t="s">
@@ -2294,10 +2299,10 @@
       </c>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
-      <c r="G18" s="3" t="s">
+      <c r="G18" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="H18" s="7" t="s">
+      <c r="H18" s="8" t="s">
         <v>39</v>
       </c>
       <c r="I18" s="2">
@@ -2316,7 +2321,7 @@
       <c r="P18" s="2">
         <v>100</v>
       </c>
-      <c r="Q18" s="9"/>
+      <c r="Q18" s="10"/>
     </row>
     <row r="19" ht="17.6" spans="1:17">
       <c r="A19" s="2" t="s">
@@ -2333,10 +2338,10 @@
       </c>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
-      <c r="G19" s="3" t="s">
+      <c r="G19" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="H19" s="3" t="s">
+      <c r="H19" s="4" t="s">
         <v>40</v>
       </c>
       <c r="I19" s="2">
@@ -2355,7 +2360,7 @@
       <c r="P19" s="2">
         <v>100</v>
       </c>
-      <c r="Q19" s="9"/>
+      <c r="Q19" s="10"/>
     </row>
     <row r="20" ht="17.6" spans="1:17">
       <c r="A20" s="2" t="s">
@@ -2372,10 +2377,10 @@
       </c>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
-      <c r="G20" s="3" t="s">
+      <c r="G20" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="H20" s="3" t="s">
+      <c r="H20" s="4" t="s">
         <v>41</v>
       </c>
       <c r="I20" s="2">
@@ -2394,7 +2399,7 @@
       <c r="P20" s="2">
         <v>100</v>
       </c>
-      <c r="Q20" s="9"/>
+      <c r="Q20" s="10"/>
     </row>
     <row r="21" ht="17.6" spans="1:17">
       <c r="A21" s="2" t="s">
@@ -2411,10 +2416,10 @@
       </c>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
-      <c r="G21" s="3" t="s">
+      <c r="G21" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="H21" s="3" t="s">
+      <c r="H21" s="4" t="s">
         <v>42</v>
       </c>
       <c r="I21" s="2">
@@ -2433,7 +2438,7 @@
       <c r="P21" s="2">
         <v>100</v>
       </c>
-      <c r="Q21" s="9"/>
+      <c r="Q21" s="10"/>
     </row>
     <row r="22" ht="17.6" spans="1:17">
       <c r="A22" s="2" t="s">
@@ -2450,10 +2455,10 @@
       </c>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
-      <c r="G22" s="3" t="s">
+      <c r="G22" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="H22" s="3" t="s">
+      <c r="H22" s="4" t="s">
         <v>43</v>
       </c>
       <c r="I22" s="2">
@@ -2472,7 +2477,7 @@
       <c r="P22" s="2">
         <v>100</v>
       </c>
-      <c r="Q22" s="9"/>
+      <c r="Q22" s="10"/>
     </row>
     <row r="23" ht="17.6" spans="1:17">
       <c r="A23" s="2" t="s">
@@ -2489,10 +2494,10 @@
       </c>
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
-      <c r="G23" s="3" t="s">
+      <c r="G23" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="H23" s="3" t="s">
+      <c r="H23" s="4" t="s">
         <v>45</v>
       </c>
       <c r="I23" s="2">
@@ -2511,7 +2516,7 @@
       <c r="P23" s="2">
         <v>75</v>
       </c>
-      <c r="Q23" s="9"/>
+      <c r="Q23" s="10"/>
     </row>
     <row r="24" ht="17.6" spans="1:17">
       <c r="A24" s="2" t="s">
@@ -2528,10 +2533,10 @@
       </c>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
-      <c r="G24" s="3" t="s">
+      <c r="G24" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="H24" s="3" t="s">
+      <c r="H24" s="4" t="s">
         <v>46</v>
       </c>
       <c r="I24" s="2">
@@ -2550,7 +2555,7 @@
       <c r="P24" s="2">
         <v>75</v>
       </c>
-      <c r="Q24" s="9"/>
+      <c r="Q24" s="10"/>
     </row>
     <row r="25" ht="17.6" spans="1:17">
       <c r="A25" s="2" t="s">
@@ -2567,10 +2572,10 @@
       </c>
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
-      <c r="G25" s="3" t="s">
+      <c r="G25" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="H25" s="3" t="s">
+      <c r="H25" s="4" t="s">
         <v>47</v>
       </c>
       <c r="I25" s="2">
@@ -2589,7 +2594,7 @@
       <c r="P25" s="2">
         <v>75</v>
       </c>
-      <c r="Q25" s="9"/>
+      <c r="Q25" s="10"/>
     </row>
     <row r="26" ht="17.6" spans="1:17">
       <c r="A26" s="2" t="s">
@@ -2606,10 +2611,10 @@
       </c>
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
-      <c r="G26" s="3" t="s">
+      <c r="G26" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="H26" s="3" t="s">
+      <c r="H26" s="4" t="s">
         <v>48</v>
       </c>
       <c r="I26" s="2">
@@ -2628,7 +2633,7 @@
       <c r="P26" s="2">
         <v>75</v>
       </c>
-      <c r="Q26" s="9"/>
+      <c r="Q26" s="10"/>
     </row>
     <row r="27" ht="17.6" spans="1:17">
       <c r="A27" s="2" t="s">
@@ -2645,10 +2650,10 @@
       </c>
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
-      <c r="G27" s="3" t="s">
+      <c r="G27" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="H27" s="3" t="s">
+      <c r="H27" s="4" t="s">
         <v>49</v>
       </c>
       <c r="I27" s="2">
@@ -2667,7 +2672,7 @@
       <c r="P27" s="2">
         <v>75</v>
       </c>
-      <c r="Q27" s="9"/>
+      <c r="Q27" s="10"/>
     </row>
     <row r="28" ht="17.6" spans="1:17">
       <c r="A28" s="2" t="s">
@@ -2684,10 +2689,10 @@
       </c>
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
-      <c r="G28" s="3" t="s">
+      <c r="G28" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="H28" s="3" t="s">
+      <c r="H28" s="4" t="s">
         <v>50</v>
       </c>
       <c r="I28" s="2">
@@ -2706,7 +2711,7 @@
       <c r="P28" s="2">
         <v>75</v>
       </c>
-      <c r="Q28" s="9"/>
+      <c r="Q28" s="10"/>
     </row>
     <row r="29" ht="17.6" spans="1:17">
       <c r="A29" s="2" t="s">
@@ -2723,10 +2728,10 @@
       </c>
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
-      <c r="G29" s="3" t="s">
+      <c r="G29" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="H29" s="3" t="s">
+      <c r="H29" s="4" t="s">
         <v>51</v>
       </c>
       <c r="I29" s="2">
@@ -2745,7 +2750,7 @@
       <c r="P29" s="2">
         <v>75</v>
       </c>
-      <c r="Q29" s="9"/>
+      <c r="Q29" s="10"/>
     </row>
     <row r="30" ht="17.6" spans="1:17">
       <c r="A30" s="2" t="s">
@@ -2762,10 +2767,10 @@
       </c>
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
-      <c r="G30" s="3" t="s">
+      <c r="G30" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="H30" s="3" t="s">
+      <c r="H30" s="4" t="s">
         <v>52</v>
       </c>
       <c r="I30" s="2">
@@ -2784,7 +2789,7 @@
       <c r="P30" s="2">
         <v>75</v>
       </c>
-      <c r="Q30" s="9"/>
+      <c r="Q30" s="10"/>
     </row>
     <row r="31" ht="17.6" spans="1:17">
       <c r="A31" s="2" t="s">
@@ -2801,10 +2806,10 @@
       </c>
       <c r="E31" s="2"/>
       <c r="F31" s="2"/>
-      <c r="G31" s="3" t="s">
+      <c r="G31" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="H31" s="3" t="s">
+      <c r="H31" s="4" t="s">
         <v>53</v>
       </c>
       <c r="I31" s="2">
@@ -2823,7 +2828,7 @@
       <c r="P31" s="2">
         <v>75</v>
       </c>
-      <c r="Q31" s="9"/>
+      <c r="Q31" s="10"/>
     </row>
     <row r="32" ht="17.6" spans="1:17">
       <c r="A32" s="2" t="s">
@@ -2840,10 +2845,10 @@
       </c>
       <c r="E32" s="2"/>
       <c r="F32" s="2"/>
-      <c r="G32" s="3" t="s">
+      <c r="G32" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="H32" s="3" t="s">
+      <c r="H32" s="4" t="s">
         <v>54</v>
       </c>
       <c r="I32" s="2">
@@ -2862,7 +2867,7 @@
       <c r="P32" s="2">
         <v>75</v>
       </c>
-      <c r="Q32" s="9"/>
+      <c r="Q32" s="10"/>
     </row>
     <row r="33" ht="17.6" spans="1:17">
       <c r="A33" s="2" t="s">
@@ -2879,10 +2884,10 @@
       </c>
       <c r="E33" s="2"/>
       <c r="F33" s="2"/>
-      <c r="G33" s="3" t="s">
+      <c r="G33" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="H33" s="3" t="s">
+      <c r="H33" s="4" t="s">
         <v>55</v>
       </c>
       <c r="I33" s="2">
@@ -2901,7 +2906,7 @@
       <c r="P33" s="2">
         <v>75</v>
       </c>
-      <c r="Q33" s="9"/>
+      <c r="Q33" s="10"/>
     </row>
     <row r="34" ht="17.6" spans="1:17">
       <c r="A34" s="2" t="s">
@@ -2918,16 +2923,16 @@
       </c>
       <c r="E34" s="2"/>
       <c r="F34" s="2"/>
-      <c r="G34" s="3" t="s">
+      <c r="G34" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="H34" s="3" t="s">
+      <c r="H34" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="I34" s="8">
+      <c r="I34" s="9">
         <v>3</v>
       </c>
-      <c r="J34" s="8"/>
+      <c r="J34" s="9"/>
       <c r="K34" s="2">
         <v>50</v>
       </c>
@@ -2940,7 +2945,7 @@
       <c r="P34" s="2">
         <v>75</v>
       </c>
-      <c r="Q34" s="9"/>
+      <c r="Q34" s="10"/>
     </row>
     <row r="35" ht="17.6" spans="1:17">
       <c r="A35" s="2" t="s">
@@ -2957,16 +2962,16 @@
       </c>
       <c r="E35" s="2"/>
       <c r="F35" s="2"/>
-      <c r="G35" s="3" t="s">
+      <c r="G35" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="H35" s="3" t="s">
+      <c r="H35" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="I35" s="8">
+      <c r="I35" s="9">
         <v>3</v>
       </c>
-      <c r="J35" s="8"/>
+      <c r="J35" s="9"/>
       <c r="K35" s="2">
         <v>50</v>
       </c>
@@ -2979,7 +2984,7 @@
       <c r="P35" s="2">
         <v>75</v>
       </c>
-      <c r="Q35" s="9"/>
+      <c r="Q35" s="10"/>
     </row>
     <row r="36" ht="17.6" spans="1:17">
       <c r="A36" s="2" t="s">
@@ -2996,16 +3001,16 @@
       </c>
       <c r="E36" s="2"/>
       <c r="F36" s="2"/>
-      <c r="G36" s="3" t="s">
+      <c r="G36" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="H36" s="3" t="s">
+      <c r="H36" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="I36" s="8">
+      <c r="I36" s="9">
         <v>3</v>
       </c>
-      <c r="J36" s="8"/>
+      <c r="J36" s="9"/>
       <c r="K36" s="2">
         <v>50</v>
       </c>
@@ -3018,7 +3023,7 @@
       <c r="P36" s="2">
         <v>75</v>
       </c>
-      <c r="Q36" s="9"/>
+      <c r="Q36" s="10"/>
     </row>
     <row r="37" ht="17.6" spans="1:17">
       <c r="A37" s="2" t="s">
@@ -3035,16 +3040,16 @@
       </c>
       <c r="E37" s="2"/>
       <c r="F37" s="2"/>
-      <c r="G37" s="3" t="s">
+      <c r="G37" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="H37" s="3" t="s">
+      <c r="H37" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="I37" s="8">
+      <c r="I37" s="9">
         <v>3</v>
       </c>
-      <c r="J37" s="8"/>
+      <c r="J37" s="9"/>
       <c r="K37" s="2">
         <v>50</v>
       </c>
@@ -3057,7 +3062,7 @@
       <c r="P37" s="2">
         <v>75</v>
       </c>
-      <c r="Q37" s="9"/>
+      <c r="Q37" s="10"/>
     </row>
     <row r="38" ht="17.6" spans="1:17">
       <c r="A38" s="2" t="s">
@@ -3074,16 +3079,16 @@
       </c>
       <c r="E38" s="2"/>
       <c r="F38" s="2"/>
-      <c r="G38" s="3" t="s">
+      <c r="G38" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="H38" s="3" t="s">
+      <c r="H38" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="I38" s="8">
+      <c r="I38" s="9">
         <v>3</v>
       </c>
-      <c r="J38" s="8"/>
+      <c r="J38" s="9"/>
       <c r="K38" s="2">
         <v>50</v>
       </c>
@@ -3096,7 +3101,7 @@
       <c r="P38" s="2">
         <v>75</v>
       </c>
-      <c r="Q38" s="9"/>
+      <c r="Q38" s="10"/>
     </row>
     <row r="39" ht="17.6" spans="1:17">
       <c r="A39" s="2" t="s">
@@ -3113,16 +3118,16 @@
       </c>
       <c r="E39" s="2"/>
       <c r="F39" s="2"/>
-      <c r="G39" s="3" t="s">
+      <c r="G39" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="H39" s="3" t="s">
+      <c r="H39" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="I39" s="8">
+      <c r="I39" s="9">
         <v>3</v>
       </c>
-      <c r="J39" s="8"/>
+      <c r="J39" s="9"/>
       <c r="K39" s="2">
         <v>50</v>
       </c>
@@ -3135,7 +3140,7 @@
       <c r="P39" s="2">
         <v>75</v>
       </c>
-      <c r="Q39" s="9"/>
+      <c r="Q39" s="10"/>
     </row>
     <row r="40" ht="17.6" spans="1:17">
       <c r="A40" s="2" t="s">
@@ -3152,10 +3157,10 @@
       </c>
       <c r="E40" s="2"/>
       <c r="F40" s="2"/>
-      <c r="G40" s="3" t="s">
+      <c r="G40" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="H40" s="3" t="s">
+      <c r="H40" s="4" t="s">
         <v>62</v>
       </c>
       <c r="I40" s="2">
@@ -3174,7 +3179,7 @@
       <c r="P40" s="2">
         <v>75</v>
       </c>
-      <c r="Q40" s="9"/>
+      <c r="Q40" s="10"/>
     </row>
     <row r="41" ht="17.6" spans="1:17">
       <c r="A41" s="2" t="s">
@@ -3191,27 +3196,27 @@
       </c>
       <c r="E41" s="2"/>
       <c r="F41" s="2"/>
-      <c r="G41" s="3" t="s">
+      <c r="G41" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="H41" s="3" t="s">
+      <c r="H41" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="I41" s="8">
+      <c r="I41" s="9">
         <v>2</v>
       </c>
-      <c r="J41" s="8"/>
+      <c r="J41" s="9"/>
       <c r="K41" s="2">
         <v>50</v>
       </c>
       <c r="L41" s="2"/>
       <c r="M41" s="2"/>
       <c r="N41" s="2"/>
-      <c r="O41" s="9"/>
+      <c r="O41" s="10"/>
       <c r="P41" s="2">
         <v>50</v>
       </c>
-      <c r="Q41" s="9"/>
+      <c r="Q41" s="10"/>
     </row>
     <row r="42" ht="17.6" spans="1:17">
       <c r="A42" s="2" t="s">
@@ -3228,27 +3233,27 @@
       </c>
       <c r="E42" s="2"/>
       <c r="F42" s="2"/>
-      <c r="G42" s="3" t="s">
+      <c r="G42" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="H42" s="3" t="s">
+      <c r="H42" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="I42" s="8">
+      <c r="I42" s="9">
         <v>2</v>
       </c>
-      <c r="J42" s="8"/>
+      <c r="J42" s="9"/>
       <c r="K42" s="2">
         <v>50</v>
       </c>
       <c r="L42" s="2"/>
       <c r="M42" s="2"/>
       <c r="N42" s="2"/>
-      <c r="O42" s="9"/>
+      <c r="O42" s="10"/>
       <c r="P42" s="2">
         <v>50</v>
       </c>
-      <c r="Q42" s="9"/>
+      <c r="Q42" s="10"/>
     </row>
     <row r="43" ht="17.6" spans="1:17">
       <c r="A43" s="2" t="s">
@@ -3265,27 +3270,27 @@
       </c>
       <c r="E43" s="2"/>
       <c r="F43" s="2"/>
-      <c r="G43" s="3" t="s">
+      <c r="G43" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="H43" s="3" t="s">
+      <c r="H43" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="I43" s="8">
+      <c r="I43" s="9">
         <v>2</v>
       </c>
-      <c r="J43" s="8"/>
+      <c r="J43" s="9"/>
       <c r="K43" s="2">
         <v>50</v>
       </c>
       <c r="L43" s="2"/>
       <c r="M43" s="2"/>
       <c r="N43" s="2"/>
-      <c r="O43" s="9"/>
+      <c r="O43" s="10"/>
       <c r="P43" s="2">
         <v>50</v>
       </c>
-      <c r="Q43" s="9"/>
+      <c r="Q43" s="10"/>
     </row>
     <row r="44" ht="17.6" spans="1:17">
       <c r="A44" s="2" t="s">
@@ -3302,10 +3307,10 @@
       </c>
       <c r="E44" s="2"/>
       <c r="F44" s="2"/>
-      <c r="G44" s="3" t="s">
+      <c r="G44" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="H44" s="4" t="s">
+      <c r="H44" s="5" t="s">
         <v>68</v>
       </c>
       <c r="I44" s="2">
@@ -3324,7 +3329,7 @@
       <c r="P44" s="2">
         <v>100</v>
       </c>
-      <c r="Q44" s="9"/>
+      <c r="Q44" s="10"/>
     </row>
     <row r="45" ht="17.6" spans="1:17">
       <c r="A45" s="2" t="s">
@@ -3341,10 +3346,10 @@
       </c>
       <c r="E45" s="2"/>
       <c r="F45" s="2"/>
-      <c r="G45" s="3" t="s">
+      <c r="G45" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="H45" s="4" t="s">
+      <c r="H45" s="5" t="s">
         <v>69</v>
       </c>
       <c r="I45" s="2">
@@ -3363,7 +3368,7 @@
       <c r="P45" s="2">
         <v>100</v>
       </c>
-      <c r="Q45" s="9"/>
+      <c r="Q45" s="10"/>
     </row>
     <row r="46" ht="17.6" spans="1:17">
       <c r="A46" s="2" t="s">
@@ -3380,10 +3385,10 @@
       </c>
       <c r="E46" s="2"/>
       <c r="F46" s="2"/>
-      <c r="G46" s="3" t="s">
+      <c r="G46" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="H46" s="4" t="s">
+      <c r="H46" s="5" t="s">
         <v>70</v>
       </c>
       <c r="I46" s="2">
@@ -3402,7 +3407,7 @@
       <c r="P46" s="2">
         <v>100</v>
       </c>
-      <c r="Q46" s="9"/>
+      <c r="Q46" s="10"/>
     </row>
     <row r="47" ht="17.6" spans="1:17">
       <c r="A47" s="2" t="s">
@@ -3419,10 +3424,10 @@
       </c>
       <c r="E47" s="2"/>
       <c r="F47" s="2"/>
-      <c r="G47" s="3" t="s">
+      <c r="G47" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="H47" s="4" t="s">
+      <c r="H47" s="5" t="s">
         <v>71</v>
       </c>
       <c r="I47" s="2">
@@ -3441,7 +3446,7 @@
       <c r="P47" s="2">
         <v>100</v>
       </c>
-      <c r="Q47" s="9"/>
+      <c r="Q47" s="10"/>
     </row>
     <row r="48" ht="17.6" spans="1:17">
       <c r="A48" s="2" t="s">
@@ -3458,10 +3463,10 @@
       </c>
       <c r="E48" s="2"/>
       <c r="F48" s="2"/>
-      <c r="G48" s="3" t="s">
+      <c r="G48" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="H48" s="4" t="s">
+      <c r="H48" s="5" t="s">
         <v>72</v>
       </c>
       <c r="I48" s="2">
@@ -3480,7 +3485,7 @@
       <c r="P48" s="2">
         <v>100</v>
       </c>
-      <c r="Q48" s="9"/>
+      <c r="Q48" s="10"/>
     </row>
     <row r="49" ht="17.6" spans="1:17">
       <c r="A49" s="2" t="s">
@@ -3497,10 +3502,10 @@
       </c>
       <c r="E49" s="2"/>
       <c r="F49" s="2"/>
-      <c r="G49" s="3" t="s">
+      <c r="G49" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="H49" s="4" t="s">
+      <c r="H49" s="5" t="s">
         <v>73</v>
       </c>
       <c r="I49" s="2">
@@ -3519,7 +3524,7 @@
       <c r="P49" s="2">
         <v>100</v>
       </c>
-      <c r="Q49" s="9"/>
+      <c r="Q49" s="10"/>
     </row>
     <row r="50" ht="17.6" spans="1:17">
       <c r="A50" s="2" t="s">
@@ -3536,10 +3541,10 @@
       </c>
       <c r="E50" s="2"/>
       <c r="F50" s="2"/>
-      <c r="G50" s="3" t="s">
+      <c r="G50" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="H50" s="4" t="s">
+      <c r="H50" s="5" t="s">
         <v>74</v>
       </c>
       <c r="I50" s="2">
@@ -3558,7 +3563,7 @@
       <c r="P50" s="2">
         <v>100</v>
       </c>
-      <c r="Q50" s="9"/>
+      <c r="Q50" s="10"/>
     </row>
     <row r="51" ht="17.6" spans="1:17">
       <c r="A51" s="2" t="s">
@@ -3575,10 +3580,10 @@
       </c>
       <c r="E51" s="2"/>
       <c r="F51" s="2"/>
-      <c r="G51" s="3" t="s">
+      <c r="G51" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="H51" s="4" t="s">
+      <c r="H51" s="5" t="s">
         <v>75</v>
       </c>
       <c r="I51" s="2">
@@ -3595,7 +3600,7 @@
       <c r="P51" s="2">
         <v>100</v>
       </c>
-      <c r="Q51" s="9"/>
+      <c r="Q51" s="10"/>
     </row>
     <row r="52" ht="17.6" spans="1:17">
       <c r="A52" s="2" t="s">
@@ -3612,10 +3617,10 @@
       </c>
       <c r="E52" s="2"/>
       <c r="F52" s="2"/>
-      <c r="G52" s="3" t="s">
+      <c r="G52" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="H52" s="4" t="s">
+      <c r="H52" s="5" t="s">
         <v>76</v>
       </c>
       <c r="I52" s="2">
@@ -3634,7 +3639,7 @@
       <c r="P52" s="2">
         <v>100</v>
       </c>
-      <c r="Q52" s="9"/>
+      <c r="Q52" s="10"/>
     </row>
     <row r="53" ht="17.6" spans="1:17">
       <c r="A53" s="2" t="s">
@@ -3651,10 +3656,10 @@
       </c>
       <c r="E53" s="2"/>
       <c r="F53" s="2"/>
-      <c r="G53" s="3" t="s">
+      <c r="G53" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="H53" s="4" t="s">
+      <c r="H53" s="5" t="s">
         <v>77</v>
       </c>
       <c r="I53" s="2">
@@ -3673,7 +3678,7 @@
       <c r="P53" s="2">
         <v>100</v>
       </c>
-      <c r="Q53" s="9"/>
+      <c r="Q53" s="10"/>
     </row>
     <row r="54" ht="17.6" spans="1:17">
       <c r="A54" s="2" t="s">
@@ -3690,10 +3695,10 @@
       </c>
       <c r="E54" s="2"/>
       <c r="F54" s="2"/>
-      <c r="G54" s="3" t="s">
+      <c r="G54" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="H54" s="4" t="s">
+      <c r="H54" s="5" t="s">
         <v>78</v>
       </c>
       <c r="I54" s="2">
@@ -3712,7 +3717,7 @@
       <c r="P54" s="2">
         <v>100</v>
       </c>
-      <c r="Q54" s="9"/>
+      <c r="Q54" s="10"/>
     </row>
     <row r="55" ht="17.6" spans="1:17">
       <c r="A55" s="2" t="s">
@@ -3729,10 +3734,10 @@
       </c>
       <c r="E55" s="2"/>
       <c r="F55" s="2"/>
-      <c r="G55" s="3" t="s">
+      <c r="G55" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="H55" s="5" t="s">
+      <c r="H55" s="6" t="s">
         <v>79</v>
       </c>
       <c r="I55" s="2">
@@ -3751,7 +3756,7 @@
       <c r="P55" s="2">
         <v>100</v>
       </c>
-      <c r="Q55" s="9"/>
+      <c r="Q55" s="10"/>
     </row>
     <row r="56" ht="17.6" spans="1:17">
       <c r="A56" s="2" t="s">
@@ -3768,10 +3773,10 @@
       </c>
       <c r="E56" s="2"/>
       <c r="F56" s="2"/>
-      <c r="G56" s="3" t="s">
+      <c r="G56" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="H56" s="5" t="s">
+      <c r="H56" s="6" t="s">
         <v>80</v>
       </c>
       <c r="I56" s="2">
@@ -3790,7 +3795,7 @@
       <c r="P56" s="2">
         <v>100</v>
       </c>
-      <c r="Q56" s="9"/>
+      <c r="Q56" s="10"/>
     </row>
     <row r="57" ht="17.6" spans="1:17">
       <c r="A57" s="2" t="s">
@@ -3807,10 +3812,10 @@
       </c>
       <c r="E57" s="2"/>
       <c r="F57" s="2"/>
-      <c r="G57" s="3" t="s">
+      <c r="G57" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="H57" s="6" t="s">
+      <c r="H57" s="7" t="s">
         <v>81</v>
       </c>
       <c r="I57" s="2">
@@ -3829,7 +3834,7 @@
       <c r="P57" s="2">
         <v>100</v>
       </c>
-      <c r="Q57" s="9"/>
+      <c r="Q57" s="10"/>
     </row>
     <row r="58" ht="17.6" spans="1:17">
       <c r="A58" s="2" t="s">
@@ -3846,10 +3851,10 @@
       </c>
       <c r="E58" s="2"/>
       <c r="F58" s="2"/>
-      <c r="G58" s="3" t="s">
+      <c r="G58" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="H58" s="5" t="s">
+      <c r="H58" s="6" t="s">
         <v>82</v>
       </c>
       <c r="I58" s="2">
@@ -3868,7 +3873,7 @@
       <c r="P58" s="2">
         <v>100</v>
       </c>
-      <c r="Q58" s="9"/>
+      <c r="Q58" s="10"/>
     </row>
     <row r="59" ht="17.6" spans="1:17">
       <c r="A59" s="2" t="s">
@@ -3885,10 +3890,10 @@
       </c>
       <c r="E59" s="2"/>
       <c r="F59" s="2"/>
-      <c r="G59" s="3" t="s">
+      <c r="G59" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="H59" s="7" t="s">
+      <c r="H59" s="8" t="s">
         <v>83</v>
       </c>
       <c r="I59" s="2">
@@ -3907,7 +3912,7 @@
       <c r="P59" s="2">
         <v>100</v>
       </c>
-      <c r="Q59" s="9"/>
+      <c r="Q59" s="10"/>
     </row>
     <row r="60" ht="17.6" spans="1:17">
       <c r="A60" s="2" t="s">
@@ -3924,10 +3929,10 @@
       </c>
       <c r="E60" s="2"/>
       <c r="F60" s="2"/>
-      <c r="G60" s="3" t="s">
+      <c r="G60" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="H60" s="7" t="s">
+      <c r="H60" s="8" t="s">
         <v>84</v>
       </c>
       <c r="I60" s="2">
@@ -3946,7 +3951,7 @@
       <c r="P60" s="2">
         <v>100</v>
       </c>
-      <c r="Q60" s="9"/>
+      <c r="Q60" s="10"/>
     </row>
     <row r="61" ht="17.6" spans="1:17">
       <c r="A61" s="2" t="s">
@@ -3963,10 +3968,10 @@
       </c>
       <c r="E61" s="2"/>
       <c r="F61" s="2"/>
-      <c r="G61" s="3" t="s">
+      <c r="G61" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="H61" s="3" t="s">
+      <c r="H61" s="4" t="s">
         <v>85</v>
       </c>
       <c r="I61" s="2">
@@ -3985,7 +3990,7 @@
       <c r="P61" s="2">
         <v>100</v>
       </c>
-      <c r="Q61" s="9"/>
+      <c r="Q61" s="10"/>
     </row>
     <row r="62" ht="17.6" spans="1:17">
       <c r="A62" s="2" t="s">
@@ -4002,10 +4007,10 @@
       </c>
       <c r="E62" s="2"/>
       <c r="F62" s="2"/>
-      <c r="G62" s="3" t="s">
+      <c r="G62" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="H62" s="3" t="s">
+      <c r="H62" s="4" t="s">
         <v>86</v>
       </c>
       <c r="I62" s="2">
@@ -4024,7 +4029,7 @@
       <c r="P62" s="2">
         <v>100</v>
       </c>
-      <c r="Q62" s="9"/>
+      <c r="Q62" s="10"/>
     </row>
     <row r="63" ht="17.6" spans="1:17">
       <c r="A63" s="2" t="s">
@@ -4041,10 +4046,10 @@
       </c>
       <c r="E63" s="2"/>
       <c r="F63" s="2"/>
-      <c r="G63" s="3" t="s">
+      <c r="G63" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="H63" s="3" t="s">
+      <c r="H63" s="4" t="s">
         <v>87</v>
       </c>
       <c r="I63" s="2">
@@ -4063,7 +4068,7 @@
       <c r="P63" s="2">
         <v>100</v>
       </c>
-      <c r="Q63" s="9"/>
+      <c r="Q63" s="10"/>
     </row>
     <row r="64" ht="17.6" spans="1:17">
       <c r="A64" s="2" t="s">
@@ -4080,10 +4085,10 @@
       </c>
       <c r="E64" s="2"/>
       <c r="F64" s="2"/>
-      <c r="G64" s="3" t="s">
+      <c r="G64" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="H64" s="3" t="s">
+      <c r="H64" s="4" t="s">
         <v>88</v>
       </c>
       <c r="I64" s="2">
@@ -4102,7 +4107,7 @@
       <c r="P64" s="2">
         <v>100</v>
       </c>
-      <c r="Q64" s="9"/>
+      <c r="Q64" s="10"/>
     </row>
     <row r="65" ht="17.6" spans="1:17">
       <c r="A65" s="2" t="s">
@@ -4119,10 +4124,10 @@
       </c>
       <c r="E65" s="2"/>
       <c r="F65" s="2"/>
-      <c r="G65" s="3" t="s">
+      <c r="G65" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="H65" s="3" t="s">
+      <c r="H65" s="4" t="s">
         <v>89</v>
       </c>
       <c r="I65" s="2">
@@ -4141,7 +4146,7 @@
       <c r="P65" s="2">
         <v>75</v>
       </c>
-      <c r="Q65" s="9"/>
+      <c r="Q65" s="10"/>
     </row>
     <row r="66" ht="17.6" spans="1:17">
       <c r="A66" s="2" t="s">
@@ -4158,10 +4163,10 @@
       </c>
       <c r="E66" s="2"/>
       <c r="F66" s="2"/>
-      <c r="G66" s="3" t="s">
+      <c r="G66" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="H66" s="3" t="s">
+      <c r="H66" s="4" t="s">
         <v>90</v>
       </c>
       <c r="I66" s="2">
@@ -4180,7 +4185,7 @@
       <c r="P66" s="2">
         <v>75</v>
       </c>
-      <c r="Q66" s="9"/>
+      <c r="Q66" s="10"/>
     </row>
     <row r="67" ht="17.6" spans="1:17">
       <c r="A67" s="2" t="s">
@@ -4197,10 +4202,10 @@
       </c>
       <c r="E67" s="2"/>
       <c r="F67" s="2"/>
-      <c r="G67" s="3" t="s">
+      <c r="G67" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="H67" s="3" t="s">
+      <c r="H67" s="4" t="s">
         <v>91</v>
       </c>
       <c r="I67" s="2">
@@ -4219,7 +4224,7 @@
       <c r="P67" s="2">
         <v>75</v>
       </c>
-      <c r="Q67" s="9"/>
+      <c r="Q67" s="10"/>
     </row>
     <row r="68" ht="17.6" spans="1:17">
       <c r="A68" s="2" t="s">
@@ -4236,10 +4241,10 @@
       </c>
       <c r="E68" s="2"/>
       <c r="F68" s="2"/>
-      <c r="G68" s="3" t="s">
+      <c r="G68" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="H68" s="3" t="s">
+      <c r="H68" s="4" t="s">
         <v>92</v>
       </c>
       <c r="I68" s="2">
@@ -4258,7 +4263,7 @@
       <c r="P68" s="2">
         <v>75</v>
       </c>
-      <c r="Q68" s="9"/>
+      <c r="Q68" s="10"/>
     </row>
     <row r="69" ht="17.6" spans="1:17">
       <c r="A69" s="2" t="s">
@@ -4275,10 +4280,10 @@
       </c>
       <c r="E69" s="2"/>
       <c r="F69" s="2"/>
-      <c r="G69" s="3" t="s">
+      <c r="G69" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="H69" s="3" t="s">
+      <c r="H69" s="4" t="s">
         <v>93</v>
       </c>
       <c r="I69" s="2">
@@ -4297,7 +4302,7 @@
       <c r="P69" s="2">
         <v>75</v>
       </c>
-      <c r="Q69" s="9"/>
+      <c r="Q69" s="10"/>
     </row>
     <row r="70" ht="17.6" spans="1:17">
       <c r="A70" s="2" t="s">
@@ -4314,10 +4319,10 @@
       </c>
       <c r="E70" s="2"/>
       <c r="F70" s="2"/>
-      <c r="G70" s="3" t="s">
+      <c r="G70" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="H70" s="3" t="s">
+      <c r="H70" s="4" t="s">
         <v>94</v>
       </c>
       <c r="I70" s="2">
@@ -4336,7 +4341,7 @@
       <c r="P70" s="2">
         <v>75</v>
       </c>
-      <c r="Q70" s="9"/>
+      <c r="Q70" s="10"/>
     </row>
     <row r="71" ht="17.6" spans="1:17">
       <c r="A71" s="2" t="s">
@@ -4353,10 +4358,10 @@
       </c>
       <c r="E71" s="2"/>
       <c r="F71" s="2"/>
-      <c r="G71" s="3" t="s">
+      <c r="G71" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="H71" s="3" t="s">
+      <c r="H71" s="4" t="s">
         <v>95</v>
       </c>
       <c r="I71" s="2">
@@ -4375,7 +4380,7 @@
       <c r="P71" s="2">
         <v>75</v>
       </c>
-      <c r="Q71" s="9"/>
+      <c r="Q71" s="10"/>
     </row>
     <row r="72" ht="17.6" spans="1:17">
       <c r="A72" s="2" t="s">
@@ -4392,10 +4397,10 @@
       </c>
       <c r="E72" s="2"/>
       <c r="F72" s="2"/>
-      <c r="G72" s="3" t="s">
+      <c r="G72" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="H72" s="3" t="s">
+      <c r="H72" s="4" t="s">
         <v>96</v>
       </c>
       <c r="I72" s="2">
@@ -4414,7 +4419,7 @@
       <c r="P72" s="2">
         <v>75</v>
       </c>
-      <c r="Q72" s="9"/>
+      <c r="Q72" s="10"/>
     </row>
     <row r="73" ht="17.6" spans="1:17">
       <c r="A73" s="2" t="s">
@@ -4431,10 +4436,10 @@
       </c>
       <c r="E73" s="2"/>
       <c r="F73" s="2"/>
-      <c r="G73" s="3" t="s">
+      <c r="G73" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="H73" s="3" t="s">
+      <c r="H73" s="4" t="s">
         <v>97</v>
       </c>
       <c r="I73" s="2">
@@ -4453,7 +4458,7 @@
       <c r="P73" s="2">
         <v>75</v>
       </c>
-      <c r="Q73" s="9"/>
+      <c r="Q73" s="10"/>
     </row>
     <row r="74" ht="17.6" spans="1:17">
       <c r="A74" s="2" t="s">
@@ -4470,10 +4475,10 @@
       </c>
       <c r="E74" s="2"/>
       <c r="F74" s="2"/>
-      <c r="G74" s="3" t="s">
+      <c r="G74" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="H74" s="3" t="s">
+      <c r="H74" s="4" t="s">
         <v>98</v>
       </c>
       <c r="I74" s="2">
@@ -4492,7 +4497,7 @@
       <c r="P74" s="2">
         <v>75</v>
       </c>
-      <c r="Q74" s="9"/>
+      <c r="Q74" s="10"/>
     </row>
     <row r="75" ht="17.6" spans="1:17">
       <c r="A75" s="2" t="s">
@@ -4509,10 +4514,10 @@
       </c>
       <c r="E75" s="2"/>
       <c r="F75" s="2"/>
-      <c r="G75" s="3" t="s">
+      <c r="G75" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="H75" s="3" t="s">
+      <c r="H75" s="4" t="s">
         <v>99</v>
       </c>
       <c r="I75" s="2">
@@ -4531,7 +4536,7 @@
       <c r="P75" s="2">
         <v>75</v>
       </c>
-      <c r="Q75" s="9"/>
+      <c r="Q75" s="10"/>
     </row>
     <row r="76" ht="17.6" spans="1:17">
       <c r="A76" s="2" t="s">
@@ -4548,10 +4553,10 @@
       </c>
       <c r="E76" s="2"/>
       <c r="F76" s="2"/>
-      <c r="G76" s="3" t="s">
+      <c r="G76" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="H76" s="3" t="s">
+      <c r="H76" s="4" t="s">
         <v>100</v>
       </c>
       <c r="I76" s="2">
@@ -4570,7 +4575,7 @@
       <c r="P76" s="2">
         <v>75</v>
       </c>
-      <c r="Q76" s="9"/>
+      <c r="Q76" s="10"/>
     </row>
     <row r="77" ht="17.6" spans="1:17">
       <c r="A77" s="2" t="s">
@@ -4587,10 +4592,10 @@
       </c>
       <c r="E77" s="2"/>
       <c r="F77" s="2"/>
-      <c r="G77" s="3" t="s">
+      <c r="G77" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="H77" s="3" t="s">
+      <c r="H77" s="4" t="s">
         <v>101</v>
       </c>
       <c r="I77" s="2">
@@ -4609,7 +4614,7 @@
       <c r="P77" s="2">
         <v>75</v>
       </c>
-      <c r="Q77" s="9"/>
+      <c r="Q77" s="10"/>
     </row>
     <row r="78" ht="17.6" spans="1:17">
       <c r="A78" s="2" t="s">
@@ -4626,10 +4631,10 @@
       </c>
       <c r="E78" s="2"/>
       <c r="F78" s="2"/>
-      <c r="G78" s="3" t="s">
+      <c r="G78" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="H78" s="3" t="s">
+      <c r="H78" s="4" t="s">
         <v>102</v>
       </c>
       <c r="I78" s="2">
@@ -4648,7 +4653,7 @@
       <c r="P78" s="2">
         <v>75</v>
       </c>
-      <c r="Q78" s="9"/>
+      <c r="Q78" s="10"/>
     </row>
     <row r="79" ht="17.6" spans="1:17">
       <c r="A79" s="2" t="s">
@@ -4665,10 +4670,10 @@
       </c>
       <c r="E79" s="2"/>
       <c r="F79" s="2"/>
-      <c r="G79" s="3" t="s">
+      <c r="G79" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="H79" s="3" t="s">
+      <c r="H79" s="4" t="s">
         <v>103</v>
       </c>
       <c r="I79" s="2">
@@ -4687,7 +4692,7 @@
       <c r="P79" s="2">
         <v>75</v>
       </c>
-      <c r="Q79" s="9"/>
+      <c r="Q79" s="10"/>
     </row>
     <row r="80" ht="17.6" spans="1:17">
       <c r="A80" s="2" t="s">
@@ -4704,10 +4709,10 @@
       </c>
       <c r="E80" s="2"/>
       <c r="F80" s="2"/>
-      <c r="G80" s="3" t="s">
+      <c r="G80" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="H80" s="3" t="s">
+      <c r="H80" s="4" t="s">
         <v>104</v>
       </c>
       <c r="I80" s="2">
@@ -4726,7 +4731,7 @@
       <c r="P80" s="2">
         <v>75</v>
       </c>
-      <c r="Q80" s="9"/>
+      <c r="Q80" s="10"/>
     </row>
     <row r="81" ht="17.6" spans="1:17">
       <c r="A81" s="2" t="s">
@@ -4743,10 +4748,10 @@
       </c>
       <c r="E81" s="2"/>
       <c r="F81" s="2"/>
-      <c r="G81" s="3" t="s">
+      <c r="G81" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="H81" s="3" t="s">
+      <c r="H81" s="4" t="s">
         <v>105</v>
       </c>
       <c r="I81" s="2">
@@ -4765,7 +4770,7 @@
       <c r="P81" s="2">
         <v>75</v>
       </c>
-      <c r="Q81" s="9"/>
+      <c r="Q81" s="10"/>
     </row>
     <row r="82" ht="17.6" spans="1:17">
       <c r="A82" s="2" t="s">
@@ -4782,10 +4787,10 @@
       </c>
       <c r="E82" s="2"/>
       <c r="F82" s="2"/>
-      <c r="G82" s="3" t="s">
+      <c r="G82" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="H82" s="3" t="s">
+      <c r="H82" s="4" t="s">
         <v>106</v>
       </c>
       <c r="I82" s="2">
@@ -4804,7 +4809,7 @@
       <c r="P82" s="2">
         <v>75</v>
       </c>
-      <c r="Q82" s="9"/>
+      <c r="Q82" s="10"/>
     </row>
     <row r="83" ht="17.6" spans="1:17">
       <c r="A83" s="2" t="s">
@@ -4821,27 +4826,27 @@
       </c>
       <c r="E83" s="2"/>
       <c r="F83" s="2"/>
-      <c r="G83" s="3" t="s">
+      <c r="G83" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="H83" s="3" t="s">
+      <c r="H83" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="I83" s="8">
+      <c r="I83" s="9">
         <v>2</v>
       </c>
-      <c r="J83" s="8"/>
+      <c r="J83" s="9"/>
       <c r="K83" s="2">
         <v>50</v>
       </c>
       <c r="L83" s="2"/>
       <c r="M83" s="2"/>
       <c r="N83" s="2"/>
-      <c r="O83" s="9"/>
+      <c r="O83" s="10"/>
       <c r="P83" s="2">
         <v>50</v>
       </c>
-      <c r="Q83" s="9"/>
+      <c r="Q83" s="10"/>
     </row>
     <row r="84" ht="17.6" spans="1:17">
       <c r="A84" s="2" t="s">
@@ -4858,27 +4863,27 @@
       </c>
       <c r="E84" s="2"/>
       <c r="F84" s="2"/>
-      <c r="G84" s="3" t="s">
+      <c r="G84" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="H84" s="3" t="s">
+      <c r="H84" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="I84" s="8">
+      <c r="I84" s="9">
         <v>2</v>
       </c>
-      <c r="J84" s="8"/>
+      <c r="J84" s="9"/>
       <c r="K84" s="2">
         <v>50</v>
       </c>
       <c r="L84" s="2"/>
       <c r="M84" s="2"/>
       <c r="N84" s="2"/>
-      <c r="O84" s="9"/>
+      <c r="O84" s="10"/>
       <c r="P84" s="2">
         <v>50</v>
       </c>
-      <c r="Q84" s="9"/>
+      <c r="Q84" s="10"/>
     </row>
     <row r="85" ht="17.6" spans="1:17">
       <c r="A85" s="2" t="s">
@@ -4895,27 +4900,27 @@
       </c>
       <c r="E85" s="2"/>
       <c r="F85" s="2"/>
-      <c r="G85" s="3" t="s">
+      <c r="G85" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="H85" s="3" t="s">
+      <c r="H85" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="I85" s="8">
+      <c r="I85" s="9">
         <v>2</v>
       </c>
-      <c r="J85" s="8"/>
+      <c r="J85" s="9"/>
       <c r="K85" s="2">
         <v>50</v>
       </c>
       <c r="L85" s="2"/>
       <c r="M85" s="2"/>
       <c r="N85" s="2"/>
-      <c r="O85" s="9"/>
+      <c r="O85" s="10"/>
       <c r="P85" s="2">
         <v>50</v>
       </c>
-      <c r="Q85" s="9"/>
+      <c r="Q85" s="10"/>
     </row>
     <row r="86" spans="1:17">
       <c r="A86" s="2" t="s">
@@ -4932,10 +4937,10 @@
       </c>
       <c r="E86" s="2"/>
       <c r="F86" s="2"/>
-      <c r="G86" s="3" t="s">
+      <c r="G86" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="H86" s="3" t="s">
+      <c r="H86" s="4" t="s">
         <v>111</v>
       </c>
       <c r="I86" s="2">

</xml_diff>

<commit_message>
fixed marksheet flow by removing formulas and fixing batches and subjects service
</commit_message>
<xml_diff>
--- a/apps/backend/public/data/ccf-ba-subjects.xlsx
+++ b/apps/backend/public/data/ccf-ba-subjects.xlsx
@@ -47,7 +47,7 @@
     <t>Specialization</t>
   </si>
   <si>
-    <t>Subject Type as per Marksheet</t>
+    <t>Subject Name as per Marksheet (also in IRP)</t>
   </si>
   <si>
     <t>Subject Code as per Marksheet</t>
@@ -1020,7 +1020,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1029,6 +1029,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1600,8 +1603,8 @@
   <sheetPr/>
   <dimension ref="A1:Q86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8"/>
@@ -1633,7 +1636,7 @@
       <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="4" t="s">
         <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
@@ -1660,7 +1663,7 @@
       <c r="P1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="11" t="s">
+      <c r="Q1" s="12" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1679,10 +1682,10 @@
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="H2" s="6" t="s">
         <v>21</v>
       </c>
       <c r="I2" s="2">
@@ -1701,7 +1704,7 @@
       <c r="P2" s="2">
         <v>100</v>
       </c>
-      <c r="Q2" s="10"/>
+      <c r="Q2" s="11"/>
     </row>
     <row r="3" ht="17.6" spans="1:17">
       <c r="A3" s="2" t="s">
@@ -1718,10 +1721,10 @@
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="H3" s="6" t="s">
         <v>22</v>
       </c>
       <c r="I3" s="2">
@@ -1740,7 +1743,7 @@
       <c r="P3" s="2">
         <v>100</v>
       </c>
-      <c r="Q3" s="10"/>
+      <c r="Q3" s="11"/>
     </row>
     <row r="4" ht="17.6" spans="1:17">
       <c r="A4" s="2" t="s">
@@ -1757,10 +1760,10 @@
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
-      <c r="G4" s="4" t="s">
+      <c r="G4" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="H4" s="6" t="s">
         <v>23</v>
       </c>
       <c r="I4" s="2">
@@ -1779,7 +1782,7 @@
       <c r="P4" s="2">
         <v>100</v>
       </c>
-      <c r="Q4" s="10"/>
+      <c r="Q4" s="11"/>
     </row>
     <row r="5" ht="17.6" spans="1:17">
       <c r="A5" s="2" t="s">
@@ -1796,10 +1799,10 @@
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
-      <c r="G5" s="4" t="s">
+      <c r="G5" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="H5" s="5" t="s">
+      <c r="H5" s="6" t="s">
         <v>24</v>
       </c>
       <c r="I5" s="2">
@@ -1818,7 +1821,7 @@
       <c r="P5" s="2">
         <v>100</v>
       </c>
-      <c r="Q5" s="10"/>
+      <c r="Q5" s="11"/>
     </row>
     <row r="6" ht="17.6" spans="1:17">
       <c r="A6" s="2" t="s">
@@ -1835,10 +1838,10 @@
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
-      <c r="G6" s="4" t="s">
+      <c r="G6" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="H6" s="5" t="s">
+      <c r="H6" s="6" t="s">
         <v>25</v>
       </c>
       <c r="I6" s="2">
@@ -1857,7 +1860,7 @@
       <c r="P6" s="2">
         <v>100</v>
       </c>
-      <c r="Q6" s="10"/>
+      <c r="Q6" s="11"/>
     </row>
     <row r="7" ht="17.6" spans="1:17">
       <c r="A7" s="2" t="s">
@@ -1874,10 +1877,10 @@
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
-      <c r="G7" s="4" t="s">
+      <c r="G7" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="H7" s="5" t="s">
+      <c r="H7" s="6" t="s">
         <v>27</v>
       </c>
       <c r="I7" s="2">
@@ -1894,7 +1897,7 @@
       <c r="P7" s="2">
         <v>100</v>
       </c>
-      <c r="Q7" s="10"/>
+      <c r="Q7" s="11"/>
     </row>
     <row r="8" ht="17.6" spans="1:17">
       <c r="A8" s="2" t="s">
@@ -1911,10 +1914,10 @@
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
-      <c r="G8" s="4" t="s">
+      <c r="G8" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="H8" s="5" t="s">
+      <c r="H8" s="6" t="s">
         <v>28</v>
       </c>
       <c r="I8" s="2">
@@ -1933,7 +1936,7 @@
       <c r="P8" s="2">
         <v>100</v>
       </c>
-      <c r="Q8" s="10"/>
+      <c r="Q8" s="11"/>
     </row>
     <row r="9" ht="17.6" spans="1:17">
       <c r="A9" s="2" t="s">
@@ -1950,10 +1953,10 @@
       </c>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
-      <c r="G9" s="4" t="s">
+      <c r="G9" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="H9" s="5" t="s">
+      <c r="H9" s="6" t="s">
         <v>29</v>
       </c>
       <c r="I9" s="2">
@@ -1970,7 +1973,7 @@
       <c r="P9" s="2">
         <v>100</v>
       </c>
-      <c r="Q9" s="10"/>
+      <c r="Q9" s="11"/>
     </row>
     <row r="10" ht="17.6" spans="1:17">
       <c r="A10" s="2" t="s">
@@ -1987,10 +1990,10 @@
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
-      <c r="G10" s="4" t="s">
+      <c r="G10" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="H10" s="5" t="s">
+      <c r="H10" s="6" t="s">
         <v>30</v>
       </c>
       <c r="I10" s="2">
@@ -2009,7 +2012,7 @@
       <c r="P10" s="2">
         <v>100</v>
       </c>
-      <c r="Q10" s="10"/>
+      <c r="Q10" s="11"/>
     </row>
     <row r="11" ht="17.6" spans="1:17">
       <c r="A11" s="2" t="s">
@@ -2026,10 +2029,10 @@
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
-      <c r="G11" s="4" t="s">
+      <c r="G11" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="H11" s="5" t="s">
+      <c r="H11" s="6" t="s">
         <v>31</v>
       </c>
       <c r="I11" s="2">
@@ -2048,7 +2051,7 @@
       <c r="P11" s="2">
         <v>100</v>
       </c>
-      <c r="Q11" s="10"/>
+      <c r="Q11" s="11"/>
     </row>
     <row r="12" ht="17.6" spans="1:17">
       <c r="A12" s="2" t="s">
@@ -2065,10 +2068,10 @@
       </c>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
-      <c r="G12" s="4" t="s">
+      <c r="G12" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="H12" s="5" t="s">
+      <c r="H12" s="6" t="s">
         <v>33</v>
       </c>
       <c r="I12" s="2">
@@ -2087,7 +2090,7 @@
       <c r="P12" s="2">
         <v>100</v>
       </c>
-      <c r="Q12" s="10"/>
+      <c r="Q12" s="11"/>
     </row>
     <row r="13" ht="17.6" spans="1:17">
       <c r="A13" s="2" t="s">
@@ -2104,10 +2107,10 @@
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
-      <c r="G13" s="4" t="s">
+      <c r="G13" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="H13" s="6" t="s">
+      <c r="H13" s="7" t="s">
         <v>34</v>
       </c>
       <c r="I13" s="2">
@@ -2126,7 +2129,7 @@
       <c r="P13" s="2">
         <v>100</v>
       </c>
-      <c r="Q13" s="10"/>
+      <c r="Q13" s="11"/>
     </row>
     <row r="14" ht="17.6" spans="1:17">
       <c r="A14" s="2" t="s">
@@ -2143,10 +2146,10 @@
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
-      <c r="G14" s="4" t="s">
+      <c r="G14" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="H14" s="6" t="s">
+      <c r="H14" s="7" t="s">
         <v>35</v>
       </c>
       <c r="I14" s="2">
@@ -2165,7 +2168,7 @@
       <c r="P14" s="2">
         <v>100</v>
       </c>
-      <c r="Q14" s="10"/>
+      <c r="Q14" s="11"/>
     </row>
     <row r="15" ht="17.6" spans="1:17">
       <c r="A15" s="2" t="s">
@@ -2182,10 +2185,10 @@
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
-      <c r="G15" s="4" t="s">
+      <c r="G15" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="H15" s="7" t="s">
+      <c r="H15" s="8" t="s">
         <v>36</v>
       </c>
       <c r="I15" s="2">
@@ -2204,7 +2207,7 @@
       <c r="P15" s="2">
         <v>100</v>
       </c>
-      <c r="Q15" s="10"/>
+      <c r="Q15" s="11"/>
     </row>
     <row r="16" ht="17.6" spans="1:17">
       <c r="A16" s="2" t="s">
@@ -2221,10 +2224,10 @@
       </c>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
-      <c r="G16" s="4" t="s">
+      <c r="G16" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="H16" s="6" t="s">
+      <c r="H16" s="7" t="s">
         <v>37</v>
       </c>
       <c r="I16" s="2">
@@ -2243,7 +2246,7 @@
       <c r="P16" s="2">
         <v>100</v>
       </c>
-      <c r="Q16" s="10"/>
+      <c r="Q16" s="11"/>
     </row>
     <row r="17" ht="17.6" spans="1:17">
       <c r="A17" s="2" t="s">
@@ -2260,10 +2263,10 @@
       </c>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
-      <c r="G17" s="4" t="s">
+      <c r="G17" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="H17" s="8" t="s">
+      <c r="H17" s="9" t="s">
         <v>38</v>
       </c>
       <c r="I17" s="2">
@@ -2282,7 +2285,7 @@
       <c r="P17" s="2">
         <v>100</v>
       </c>
-      <c r="Q17" s="10"/>
+      <c r="Q17" s="11"/>
     </row>
     <row r="18" ht="17.6" spans="1:17">
       <c r="A18" s="2" t="s">
@@ -2299,10 +2302,10 @@
       </c>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
-      <c r="G18" s="4" t="s">
+      <c r="G18" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="H18" s="8" t="s">
+      <c r="H18" s="9" t="s">
         <v>39</v>
       </c>
       <c r="I18" s="2">
@@ -2321,7 +2324,7 @@
       <c r="P18" s="2">
         <v>100</v>
       </c>
-      <c r="Q18" s="10"/>
+      <c r="Q18" s="11"/>
     </row>
     <row r="19" ht="17.6" spans="1:17">
       <c r="A19" s="2" t="s">
@@ -2338,10 +2341,10 @@
       </c>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
-      <c r="G19" s="4" t="s">
+      <c r="G19" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="H19" s="4" t="s">
+      <c r="H19" s="5" t="s">
         <v>40</v>
       </c>
       <c r="I19" s="2">
@@ -2360,7 +2363,7 @@
       <c r="P19" s="2">
         <v>100</v>
       </c>
-      <c r="Q19" s="10"/>
+      <c r="Q19" s="11"/>
     </row>
     <row r="20" ht="17.6" spans="1:17">
       <c r="A20" s="2" t="s">
@@ -2377,10 +2380,10 @@
       </c>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
-      <c r="G20" s="4" t="s">
+      <c r="G20" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="H20" s="4" t="s">
+      <c r="H20" s="5" t="s">
         <v>41</v>
       </c>
       <c r="I20" s="2">
@@ -2399,7 +2402,7 @@
       <c r="P20" s="2">
         <v>100</v>
       </c>
-      <c r="Q20" s="10"/>
+      <c r="Q20" s="11"/>
     </row>
     <row r="21" ht="17.6" spans="1:17">
       <c r="A21" s="2" t="s">
@@ -2416,10 +2419,10 @@
       </c>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
-      <c r="G21" s="4" t="s">
+      <c r="G21" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="H21" s="4" t="s">
+      <c r="H21" s="5" t="s">
         <v>42</v>
       </c>
       <c r="I21" s="2">
@@ -2438,7 +2441,7 @@
       <c r="P21" s="2">
         <v>100</v>
       </c>
-      <c r="Q21" s="10"/>
+      <c r="Q21" s="11"/>
     </row>
     <row r="22" ht="17.6" spans="1:17">
       <c r="A22" s="2" t="s">
@@ -2455,10 +2458,10 @@
       </c>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
-      <c r="G22" s="4" t="s">
+      <c r="G22" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="H22" s="4" t="s">
+      <c r="H22" s="5" t="s">
         <v>43</v>
       </c>
       <c r="I22" s="2">
@@ -2477,7 +2480,7 @@
       <c r="P22" s="2">
         <v>100</v>
       </c>
-      <c r="Q22" s="10"/>
+      <c r="Q22" s="11"/>
     </row>
     <row r="23" ht="17.6" spans="1:17">
       <c r="A23" s="2" t="s">
@@ -2494,10 +2497,10 @@
       </c>
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
-      <c r="G23" s="4" t="s">
+      <c r="G23" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="H23" s="4" t="s">
+      <c r="H23" s="5" t="s">
         <v>45</v>
       </c>
       <c r="I23" s="2">
@@ -2516,7 +2519,7 @@
       <c r="P23" s="2">
         <v>75</v>
       </c>
-      <c r="Q23" s="10"/>
+      <c r="Q23" s="11"/>
     </row>
     <row r="24" ht="17.6" spans="1:17">
       <c r="A24" s="2" t="s">
@@ -2533,10 +2536,10 @@
       </c>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
-      <c r="G24" s="4" t="s">
+      <c r="G24" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="H24" s="4" t="s">
+      <c r="H24" s="5" t="s">
         <v>46</v>
       </c>
       <c r="I24" s="2">
@@ -2555,7 +2558,7 @@
       <c r="P24" s="2">
         <v>75</v>
       </c>
-      <c r="Q24" s="10"/>
+      <c r="Q24" s="11"/>
     </row>
     <row r="25" ht="17.6" spans="1:17">
       <c r="A25" s="2" t="s">
@@ -2572,10 +2575,10 @@
       </c>
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
-      <c r="G25" s="4" t="s">
+      <c r="G25" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="H25" s="4" t="s">
+      <c r="H25" s="5" t="s">
         <v>47</v>
       </c>
       <c r="I25" s="2">
@@ -2594,7 +2597,7 @@
       <c r="P25" s="2">
         <v>75</v>
       </c>
-      <c r="Q25" s="10"/>
+      <c r="Q25" s="11"/>
     </row>
     <row r="26" ht="17.6" spans="1:17">
       <c r="A26" s="2" t="s">
@@ -2611,10 +2614,10 @@
       </c>
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
-      <c r="G26" s="4" t="s">
+      <c r="G26" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="H26" s="4" t="s">
+      <c r="H26" s="5" t="s">
         <v>48</v>
       </c>
       <c r="I26" s="2">
@@ -2633,7 +2636,7 @@
       <c r="P26" s="2">
         <v>75</v>
       </c>
-      <c r="Q26" s="10"/>
+      <c r="Q26" s="11"/>
     </row>
     <row r="27" ht="17.6" spans="1:17">
       <c r="A27" s="2" t="s">
@@ -2650,10 +2653,10 @@
       </c>
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
-      <c r="G27" s="4" t="s">
+      <c r="G27" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="H27" s="4" t="s">
+      <c r="H27" s="5" t="s">
         <v>49</v>
       </c>
       <c r="I27" s="2">
@@ -2672,7 +2675,7 @@
       <c r="P27" s="2">
         <v>75</v>
       </c>
-      <c r="Q27" s="10"/>
+      <c r="Q27" s="11"/>
     </row>
     <row r="28" ht="17.6" spans="1:17">
       <c r="A28" s="2" t="s">
@@ -2689,10 +2692,10 @@
       </c>
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
-      <c r="G28" s="4" t="s">
+      <c r="G28" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="H28" s="4" t="s">
+      <c r="H28" s="5" t="s">
         <v>50</v>
       </c>
       <c r="I28" s="2">
@@ -2711,7 +2714,7 @@
       <c r="P28" s="2">
         <v>75</v>
       </c>
-      <c r="Q28" s="10"/>
+      <c r="Q28" s="11"/>
     </row>
     <row r="29" ht="17.6" spans="1:17">
       <c r="A29" s="2" t="s">
@@ -2728,10 +2731,10 @@
       </c>
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
-      <c r="G29" s="4" t="s">
+      <c r="G29" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="H29" s="4" t="s">
+      <c r="H29" s="5" t="s">
         <v>51</v>
       </c>
       <c r="I29" s="2">
@@ -2750,7 +2753,7 @@
       <c r="P29" s="2">
         <v>75</v>
       </c>
-      <c r="Q29" s="10"/>
+      <c r="Q29" s="11"/>
     </row>
     <row r="30" ht="17.6" spans="1:17">
       <c r="A30" s="2" t="s">
@@ -2767,10 +2770,10 @@
       </c>
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
-      <c r="G30" s="4" t="s">
+      <c r="G30" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="H30" s="4" t="s">
+      <c r="H30" s="5" t="s">
         <v>52</v>
       </c>
       <c r="I30" s="2">
@@ -2789,7 +2792,7 @@
       <c r="P30" s="2">
         <v>75</v>
       </c>
-      <c r="Q30" s="10"/>
+      <c r="Q30" s="11"/>
     </row>
     <row r="31" ht="17.6" spans="1:17">
       <c r="A31" s="2" t="s">
@@ -2806,10 +2809,10 @@
       </c>
       <c r="E31" s="2"/>
       <c r="F31" s="2"/>
-      <c r="G31" s="4" t="s">
+      <c r="G31" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="H31" s="4" t="s">
+      <c r="H31" s="5" t="s">
         <v>53</v>
       </c>
       <c r="I31" s="2">
@@ -2828,7 +2831,7 @@
       <c r="P31" s="2">
         <v>75</v>
       </c>
-      <c r="Q31" s="10"/>
+      <c r="Q31" s="11"/>
     </row>
     <row r="32" ht="17.6" spans="1:17">
       <c r="A32" s="2" t="s">
@@ -2845,10 +2848,10 @@
       </c>
       <c r="E32" s="2"/>
       <c r="F32" s="2"/>
-      <c r="G32" s="4" t="s">
+      <c r="G32" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="H32" s="4" t="s">
+      <c r="H32" s="5" t="s">
         <v>54</v>
       </c>
       <c r="I32" s="2">
@@ -2867,7 +2870,7 @@
       <c r="P32" s="2">
         <v>75</v>
       </c>
-      <c r="Q32" s="10"/>
+      <c r="Q32" s="11"/>
     </row>
     <row r="33" ht="17.6" spans="1:17">
       <c r="A33" s="2" t="s">
@@ -2884,10 +2887,10 @@
       </c>
       <c r="E33" s="2"/>
       <c r="F33" s="2"/>
-      <c r="G33" s="4" t="s">
+      <c r="G33" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="H33" s="4" t="s">
+      <c r="H33" s="5" t="s">
         <v>55</v>
       </c>
       <c r="I33" s="2">
@@ -2906,7 +2909,7 @@
       <c r="P33" s="2">
         <v>75</v>
       </c>
-      <c r="Q33" s="10"/>
+      <c r="Q33" s="11"/>
     </row>
     <row r="34" ht="17.6" spans="1:17">
       <c r="A34" s="2" t="s">
@@ -2923,16 +2926,16 @@
       </c>
       <c r="E34" s="2"/>
       <c r="F34" s="2"/>
-      <c r="G34" s="4" t="s">
+      <c r="G34" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="H34" s="4" t="s">
+      <c r="H34" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="I34" s="9">
+      <c r="I34" s="10">
         <v>3</v>
       </c>
-      <c r="J34" s="9"/>
+      <c r="J34" s="10"/>
       <c r="K34" s="2">
         <v>50</v>
       </c>
@@ -2945,7 +2948,7 @@
       <c r="P34" s="2">
         <v>75</v>
       </c>
-      <c r="Q34" s="10"/>
+      <c r="Q34" s="11"/>
     </row>
     <row r="35" ht="17.6" spans="1:17">
       <c r="A35" s="2" t="s">
@@ -2962,16 +2965,16 @@
       </c>
       <c r="E35" s="2"/>
       <c r="F35" s="2"/>
-      <c r="G35" s="4" t="s">
+      <c r="G35" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="H35" s="4" t="s">
+      <c r="H35" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="I35" s="9">
+      <c r="I35" s="10">
         <v>3</v>
       </c>
-      <c r="J35" s="9"/>
+      <c r="J35" s="10"/>
       <c r="K35" s="2">
         <v>50</v>
       </c>
@@ -2984,7 +2987,7 @@
       <c r="P35" s="2">
         <v>75</v>
       </c>
-      <c r="Q35" s="10"/>
+      <c r="Q35" s="11"/>
     </row>
     <row r="36" ht="17.6" spans="1:17">
       <c r="A36" s="2" t="s">
@@ -3001,16 +3004,16 @@
       </c>
       <c r="E36" s="2"/>
       <c r="F36" s="2"/>
-      <c r="G36" s="4" t="s">
+      <c r="G36" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="H36" s="4" t="s">
+      <c r="H36" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="I36" s="9">
+      <c r="I36" s="10">
         <v>3</v>
       </c>
-      <c r="J36" s="9"/>
+      <c r="J36" s="10"/>
       <c r="K36" s="2">
         <v>50</v>
       </c>
@@ -3023,7 +3026,7 @@
       <c r="P36" s="2">
         <v>75</v>
       </c>
-      <c r="Q36" s="10"/>
+      <c r="Q36" s="11"/>
     </row>
     <row r="37" ht="17.6" spans="1:17">
       <c r="A37" s="2" t="s">
@@ -3040,16 +3043,16 @@
       </c>
       <c r="E37" s="2"/>
       <c r="F37" s="2"/>
-      <c r="G37" s="4" t="s">
+      <c r="G37" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="H37" s="4" t="s">
+      <c r="H37" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="I37" s="9">
+      <c r="I37" s="10">
         <v>3</v>
       </c>
-      <c r="J37" s="9"/>
+      <c r="J37" s="10"/>
       <c r="K37" s="2">
         <v>50</v>
       </c>
@@ -3062,7 +3065,7 @@
       <c r="P37" s="2">
         <v>75</v>
       </c>
-      <c r="Q37" s="10"/>
+      <c r="Q37" s="11"/>
     </row>
     <row r="38" ht="17.6" spans="1:17">
       <c r="A38" s="2" t="s">
@@ -3079,16 +3082,16 @@
       </c>
       <c r="E38" s="2"/>
       <c r="F38" s="2"/>
-      <c r="G38" s="4" t="s">
+      <c r="G38" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="H38" s="4" t="s">
+      <c r="H38" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="I38" s="9">
+      <c r="I38" s="10">
         <v>3</v>
       </c>
-      <c r="J38" s="9"/>
+      <c r="J38" s="10"/>
       <c r="K38" s="2">
         <v>50</v>
       </c>
@@ -3101,7 +3104,7 @@
       <c r="P38" s="2">
         <v>75</v>
       </c>
-      <c r="Q38" s="10"/>
+      <c r="Q38" s="11"/>
     </row>
     <row r="39" ht="17.6" spans="1:17">
       <c r="A39" s="2" t="s">
@@ -3118,16 +3121,16 @@
       </c>
       <c r="E39" s="2"/>
       <c r="F39" s="2"/>
-      <c r="G39" s="4" t="s">
+      <c r="G39" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="H39" s="4" t="s">
+      <c r="H39" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="I39" s="9">
+      <c r="I39" s="10">
         <v>3</v>
       </c>
-      <c r="J39" s="9"/>
+      <c r="J39" s="10"/>
       <c r="K39" s="2">
         <v>50</v>
       </c>
@@ -3140,7 +3143,7 @@
       <c r="P39" s="2">
         <v>75</v>
       </c>
-      <c r="Q39" s="10"/>
+      <c r="Q39" s="11"/>
     </row>
     <row r="40" ht="17.6" spans="1:17">
       <c r="A40" s="2" t="s">
@@ -3157,10 +3160,10 @@
       </c>
       <c r="E40" s="2"/>
       <c r="F40" s="2"/>
-      <c r="G40" s="4" t="s">
+      <c r="G40" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="H40" s="4" t="s">
+      <c r="H40" s="5" t="s">
         <v>62</v>
       </c>
       <c r="I40" s="2">
@@ -3179,7 +3182,7 @@
       <c r="P40" s="2">
         <v>75</v>
       </c>
-      <c r="Q40" s="10"/>
+      <c r="Q40" s="11"/>
     </row>
     <row r="41" ht="17.6" spans="1:17">
       <c r="A41" s="2" t="s">
@@ -3196,27 +3199,27 @@
       </c>
       <c r="E41" s="2"/>
       <c r="F41" s="2"/>
-      <c r="G41" s="4" t="s">
+      <c r="G41" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="H41" s="4" t="s">
+      <c r="H41" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="I41" s="9">
+      <c r="I41" s="10">
         <v>2</v>
       </c>
-      <c r="J41" s="9"/>
+      <c r="J41" s="10"/>
       <c r="K41" s="2">
         <v>50</v>
       </c>
       <c r="L41" s="2"/>
       <c r="M41" s="2"/>
       <c r="N41" s="2"/>
-      <c r="O41" s="10"/>
+      <c r="O41" s="11"/>
       <c r="P41" s="2">
         <v>50</v>
       </c>
-      <c r="Q41" s="10"/>
+      <c r="Q41" s="11"/>
     </row>
     <row r="42" ht="17.6" spans="1:17">
       <c r="A42" s="2" t="s">
@@ -3233,27 +3236,27 @@
       </c>
       <c r="E42" s="2"/>
       <c r="F42" s="2"/>
-      <c r="G42" s="4" t="s">
+      <c r="G42" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="H42" s="4" t="s">
+      <c r="H42" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="I42" s="9">
+      <c r="I42" s="10">
         <v>2</v>
       </c>
-      <c r="J42" s="9"/>
+      <c r="J42" s="10"/>
       <c r="K42" s="2">
         <v>50</v>
       </c>
       <c r="L42" s="2"/>
       <c r="M42" s="2"/>
       <c r="N42" s="2"/>
-      <c r="O42" s="10"/>
+      <c r="O42" s="11"/>
       <c r="P42" s="2">
         <v>50</v>
       </c>
-      <c r="Q42" s="10"/>
+      <c r="Q42" s="11"/>
     </row>
     <row r="43" ht="17.6" spans="1:17">
       <c r="A43" s="2" t="s">
@@ -3270,27 +3273,27 @@
       </c>
       <c r="E43" s="2"/>
       <c r="F43" s="2"/>
-      <c r="G43" s="4" t="s">
+      <c r="G43" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="H43" s="4" t="s">
+      <c r="H43" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="I43" s="9">
+      <c r="I43" s="10">
         <v>2</v>
       </c>
-      <c r="J43" s="9"/>
+      <c r="J43" s="10"/>
       <c r="K43" s="2">
         <v>50</v>
       </c>
       <c r="L43" s="2"/>
       <c r="M43" s="2"/>
       <c r="N43" s="2"/>
-      <c r="O43" s="10"/>
+      <c r="O43" s="11"/>
       <c r="P43" s="2">
         <v>50</v>
       </c>
-      <c r="Q43" s="10"/>
+      <c r="Q43" s="11"/>
     </row>
     <row r="44" ht="17.6" spans="1:17">
       <c r="A44" s="2" t="s">
@@ -3307,10 +3310,10 @@
       </c>
       <c r="E44" s="2"/>
       <c r="F44" s="2"/>
-      <c r="G44" s="4" t="s">
+      <c r="G44" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="H44" s="5" t="s">
+      <c r="H44" s="6" t="s">
         <v>68</v>
       </c>
       <c r="I44" s="2">
@@ -3329,7 +3332,7 @@
       <c r="P44" s="2">
         <v>100</v>
       </c>
-      <c r="Q44" s="10"/>
+      <c r="Q44" s="11"/>
     </row>
     <row r="45" ht="17.6" spans="1:17">
       <c r="A45" s="2" t="s">
@@ -3346,10 +3349,10 @@
       </c>
       <c r="E45" s="2"/>
       <c r="F45" s="2"/>
-      <c r="G45" s="4" t="s">
+      <c r="G45" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="H45" s="5" t="s">
+      <c r="H45" s="6" t="s">
         <v>69</v>
       </c>
       <c r="I45" s="2">
@@ -3368,7 +3371,7 @@
       <c r="P45" s="2">
         <v>100</v>
       </c>
-      <c r="Q45" s="10"/>
+      <c r="Q45" s="11"/>
     </row>
     <row r="46" ht="17.6" spans="1:17">
       <c r="A46" s="2" t="s">
@@ -3385,10 +3388,10 @@
       </c>
       <c r="E46" s="2"/>
       <c r="F46" s="2"/>
-      <c r="G46" s="4" t="s">
+      <c r="G46" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="H46" s="5" t="s">
+      <c r="H46" s="6" t="s">
         <v>70</v>
       </c>
       <c r="I46" s="2">
@@ -3407,7 +3410,7 @@
       <c r="P46" s="2">
         <v>100</v>
       </c>
-      <c r="Q46" s="10"/>
+      <c r="Q46" s="11"/>
     </row>
     <row r="47" ht="17.6" spans="1:17">
       <c r="A47" s="2" t="s">
@@ -3424,10 +3427,10 @@
       </c>
       <c r="E47" s="2"/>
       <c r="F47" s="2"/>
-      <c r="G47" s="4" t="s">
+      <c r="G47" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="H47" s="5" t="s">
+      <c r="H47" s="6" t="s">
         <v>71</v>
       </c>
       <c r="I47" s="2">
@@ -3446,7 +3449,7 @@
       <c r="P47" s="2">
         <v>100</v>
       </c>
-      <c r="Q47" s="10"/>
+      <c r="Q47" s="11"/>
     </row>
     <row r="48" ht="17.6" spans="1:17">
       <c r="A48" s="2" t="s">
@@ -3463,10 +3466,10 @@
       </c>
       <c r="E48" s="2"/>
       <c r="F48" s="2"/>
-      <c r="G48" s="4" t="s">
+      <c r="G48" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="H48" s="5" t="s">
+      <c r="H48" s="6" t="s">
         <v>72</v>
       </c>
       <c r="I48" s="2">
@@ -3485,7 +3488,7 @@
       <c r="P48" s="2">
         <v>100</v>
       </c>
-      <c r="Q48" s="10"/>
+      <c r="Q48" s="11"/>
     </row>
     <row r="49" ht="17.6" spans="1:17">
       <c r="A49" s="2" t="s">
@@ -3502,10 +3505,10 @@
       </c>
       <c r="E49" s="2"/>
       <c r="F49" s="2"/>
-      <c r="G49" s="4" t="s">
+      <c r="G49" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="H49" s="5" t="s">
+      <c r="H49" s="6" t="s">
         <v>73</v>
       </c>
       <c r="I49" s="2">
@@ -3524,7 +3527,7 @@
       <c r="P49" s="2">
         <v>100</v>
       </c>
-      <c r="Q49" s="10"/>
+      <c r="Q49" s="11"/>
     </row>
     <row r="50" ht="17.6" spans="1:17">
       <c r="A50" s="2" t="s">
@@ -3541,10 +3544,10 @@
       </c>
       <c r="E50" s="2"/>
       <c r="F50" s="2"/>
-      <c r="G50" s="4" t="s">
+      <c r="G50" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="H50" s="5" t="s">
+      <c r="H50" s="6" t="s">
         <v>74</v>
       </c>
       <c r="I50" s="2">
@@ -3563,7 +3566,7 @@
       <c r="P50" s="2">
         <v>100</v>
       </c>
-      <c r="Q50" s="10"/>
+      <c r="Q50" s="11"/>
     </row>
     <row r="51" ht="17.6" spans="1:17">
       <c r="A51" s="2" t="s">
@@ -3580,10 +3583,10 @@
       </c>
       <c r="E51" s="2"/>
       <c r="F51" s="2"/>
-      <c r="G51" s="4" t="s">
+      <c r="G51" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="H51" s="5" t="s">
+      <c r="H51" s="6" t="s">
         <v>75</v>
       </c>
       <c r="I51" s="2">
@@ -3600,7 +3603,7 @@
       <c r="P51" s="2">
         <v>100</v>
       </c>
-      <c r="Q51" s="10"/>
+      <c r="Q51" s="11"/>
     </row>
     <row r="52" ht="17.6" spans="1:17">
       <c r="A52" s="2" t="s">
@@ -3617,10 +3620,10 @@
       </c>
       <c r="E52" s="2"/>
       <c r="F52" s="2"/>
-      <c r="G52" s="4" t="s">
+      <c r="G52" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="H52" s="5" t="s">
+      <c r="H52" s="6" t="s">
         <v>76</v>
       </c>
       <c r="I52" s="2">
@@ -3639,7 +3642,7 @@
       <c r="P52" s="2">
         <v>100</v>
       </c>
-      <c r="Q52" s="10"/>
+      <c r="Q52" s="11"/>
     </row>
     <row r="53" ht="17.6" spans="1:17">
       <c r="A53" s="2" t="s">
@@ -3656,10 +3659,10 @@
       </c>
       <c r="E53" s="2"/>
       <c r="F53" s="2"/>
-      <c r="G53" s="4" t="s">
+      <c r="G53" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="H53" s="5" t="s">
+      <c r="H53" s="6" t="s">
         <v>77</v>
       </c>
       <c r="I53" s="2">
@@ -3678,7 +3681,7 @@
       <c r="P53" s="2">
         <v>100</v>
       </c>
-      <c r="Q53" s="10"/>
+      <c r="Q53" s="11"/>
     </row>
     <row r="54" ht="17.6" spans="1:17">
       <c r="A54" s="2" t="s">
@@ -3695,10 +3698,10 @@
       </c>
       <c r="E54" s="2"/>
       <c r="F54" s="2"/>
-      <c r="G54" s="4" t="s">
+      <c r="G54" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="H54" s="5" t="s">
+      <c r="H54" s="6" t="s">
         <v>78</v>
       </c>
       <c r="I54" s="2">
@@ -3717,7 +3720,7 @@
       <c r="P54" s="2">
         <v>100</v>
       </c>
-      <c r="Q54" s="10"/>
+      <c r="Q54" s="11"/>
     </row>
     <row r="55" ht="17.6" spans="1:17">
       <c r="A55" s="2" t="s">
@@ -3734,10 +3737,10 @@
       </c>
       <c r="E55" s="2"/>
       <c r="F55" s="2"/>
-      <c r="G55" s="4" t="s">
+      <c r="G55" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="H55" s="6" t="s">
+      <c r="H55" s="7" t="s">
         <v>79</v>
       </c>
       <c r="I55" s="2">
@@ -3756,7 +3759,7 @@
       <c r="P55" s="2">
         <v>100</v>
       </c>
-      <c r="Q55" s="10"/>
+      <c r="Q55" s="11"/>
     </row>
     <row r="56" ht="17.6" spans="1:17">
       <c r="A56" s="2" t="s">
@@ -3773,10 +3776,10 @@
       </c>
       <c r="E56" s="2"/>
       <c r="F56" s="2"/>
-      <c r="G56" s="4" t="s">
+      <c r="G56" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="H56" s="6" t="s">
+      <c r="H56" s="7" t="s">
         <v>80</v>
       </c>
       <c r="I56" s="2">
@@ -3795,7 +3798,7 @@
       <c r="P56" s="2">
         <v>100</v>
       </c>
-      <c r="Q56" s="10"/>
+      <c r="Q56" s="11"/>
     </row>
     <row r="57" ht="17.6" spans="1:17">
       <c r="A57" s="2" t="s">
@@ -3812,10 +3815,10 @@
       </c>
       <c r="E57" s="2"/>
       <c r="F57" s="2"/>
-      <c r="G57" s="4" t="s">
+      <c r="G57" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="H57" s="7" t="s">
+      <c r="H57" s="8" t="s">
         <v>81</v>
       </c>
       <c r="I57" s="2">
@@ -3834,7 +3837,7 @@
       <c r="P57" s="2">
         <v>100</v>
       </c>
-      <c r="Q57" s="10"/>
+      <c r="Q57" s="11"/>
     </row>
     <row r="58" ht="17.6" spans="1:17">
       <c r="A58" s="2" t="s">
@@ -3851,10 +3854,10 @@
       </c>
       <c r="E58" s="2"/>
       <c r="F58" s="2"/>
-      <c r="G58" s="4" t="s">
+      <c r="G58" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="H58" s="6" t="s">
+      <c r="H58" s="7" t="s">
         <v>82</v>
       </c>
       <c r="I58" s="2">
@@ -3873,7 +3876,7 @@
       <c r="P58" s="2">
         <v>100</v>
       </c>
-      <c r="Q58" s="10"/>
+      <c r="Q58" s="11"/>
     </row>
     <row r="59" ht="17.6" spans="1:17">
       <c r="A59" s="2" t="s">
@@ -3890,10 +3893,10 @@
       </c>
       <c r="E59" s="2"/>
       <c r="F59" s="2"/>
-      <c r="G59" s="4" t="s">
+      <c r="G59" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="H59" s="8" t="s">
+      <c r="H59" s="9" t="s">
         <v>83</v>
       </c>
       <c r="I59" s="2">
@@ -3912,7 +3915,7 @@
       <c r="P59" s="2">
         <v>100</v>
       </c>
-      <c r="Q59" s="10"/>
+      <c r="Q59" s="11"/>
     </row>
     <row r="60" ht="17.6" spans="1:17">
       <c r="A60" s="2" t="s">
@@ -3929,10 +3932,10 @@
       </c>
       <c r="E60" s="2"/>
       <c r="F60" s="2"/>
-      <c r="G60" s="4" t="s">
+      <c r="G60" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="H60" s="8" t="s">
+      <c r="H60" s="9" t="s">
         <v>84</v>
       </c>
       <c r="I60" s="2">
@@ -3951,7 +3954,7 @@
       <c r="P60" s="2">
         <v>100</v>
       </c>
-      <c r="Q60" s="10"/>
+      <c r="Q60" s="11"/>
     </row>
     <row r="61" ht="17.6" spans="1:17">
       <c r="A61" s="2" t="s">
@@ -3968,10 +3971,10 @@
       </c>
       <c r="E61" s="2"/>
       <c r="F61" s="2"/>
-      <c r="G61" s="4" t="s">
+      <c r="G61" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="H61" s="4" t="s">
+      <c r="H61" s="5" t="s">
         <v>85</v>
       </c>
       <c r="I61" s="2">
@@ -3990,7 +3993,7 @@
       <c r="P61" s="2">
         <v>100</v>
       </c>
-      <c r="Q61" s="10"/>
+      <c r="Q61" s="11"/>
     </row>
     <row r="62" ht="17.6" spans="1:17">
       <c r="A62" s="2" t="s">
@@ -4007,10 +4010,10 @@
       </c>
       <c r="E62" s="2"/>
       <c r="F62" s="2"/>
-      <c r="G62" s="4" t="s">
+      <c r="G62" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="H62" s="4" t="s">
+      <c r="H62" s="5" t="s">
         <v>86</v>
       </c>
       <c r="I62" s="2">
@@ -4029,7 +4032,7 @@
       <c r="P62" s="2">
         <v>100</v>
       </c>
-      <c r="Q62" s="10"/>
+      <c r="Q62" s="11"/>
     </row>
     <row r="63" ht="17.6" spans="1:17">
       <c r="A63" s="2" t="s">
@@ -4046,10 +4049,10 @@
       </c>
       <c r="E63" s="2"/>
       <c r="F63" s="2"/>
-      <c r="G63" s="4" t="s">
+      <c r="G63" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="H63" s="4" t="s">
+      <c r="H63" s="5" t="s">
         <v>87</v>
       </c>
       <c r="I63" s="2">
@@ -4068,7 +4071,7 @@
       <c r="P63" s="2">
         <v>100</v>
       </c>
-      <c r="Q63" s="10"/>
+      <c r="Q63" s="11"/>
     </row>
     <row r="64" ht="17.6" spans="1:17">
       <c r="A64" s="2" t="s">
@@ -4085,10 +4088,10 @@
       </c>
       <c r="E64" s="2"/>
       <c r="F64" s="2"/>
-      <c r="G64" s="4" t="s">
+      <c r="G64" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="H64" s="4" t="s">
+      <c r="H64" s="5" t="s">
         <v>88</v>
       </c>
       <c r="I64" s="2">
@@ -4107,7 +4110,7 @@
       <c r="P64" s="2">
         <v>100</v>
       </c>
-      <c r="Q64" s="10"/>
+      <c r="Q64" s="11"/>
     </row>
     <row r="65" ht="17.6" spans="1:17">
       <c r="A65" s="2" t="s">
@@ -4124,10 +4127,10 @@
       </c>
       <c r="E65" s="2"/>
       <c r="F65" s="2"/>
-      <c r="G65" s="4" t="s">
+      <c r="G65" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="H65" s="4" t="s">
+      <c r="H65" s="5" t="s">
         <v>89</v>
       </c>
       <c r="I65" s="2">
@@ -4146,7 +4149,7 @@
       <c r="P65" s="2">
         <v>75</v>
       </c>
-      <c r="Q65" s="10"/>
+      <c r="Q65" s="11"/>
     </row>
     <row r="66" ht="17.6" spans="1:17">
       <c r="A66" s="2" t="s">
@@ -4163,10 +4166,10 @@
       </c>
       <c r="E66" s="2"/>
       <c r="F66" s="2"/>
-      <c r="G66" s="4" t="s">
+      <c r="G66" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="H66" s="4" t="s">
+      <c r="H66" s="5" t="s">
         <v>90</v>
       </c>
       <c r="I66" s="2">
@@ -4185,7 +4188,7 @@
       <c r="P66" s="2">
         <v>75</v>
       </c>
-      <c r="Q66" s="10"/>
+      <c r="Q66" s="11"/>
     </row>
     <row r="67" ht="17.6" spans="1:17">
       <c r="A67" s="2" t="s">
@@ -4202,10 +4205,10 @@
       </c>
       <c r="E67" s="2"/>
       <c r="F67" s="2"/>
-      <c r="G67" s="4" t="s">
+      <c r="G67" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="H67" s="4" t="s">
+      <c r="H67" s="5" t="s">
         <v>91</v>
       </c>
       <c r="I67" s="2">
@@ -4224,7 +4227,7 @@
       <c r="P67" s="2">
         <v>75</v>
       </c>
-      <c r="Q67" s="10"/>
+      <c r="Q67" s="11"/>
     </row>
     <row r="68" ht="17.6" spans="1:17">
       <c r="A68" s="2" t="s">
@@ -4241,10 +4244,10 @@
       </c>
       <c r="E68" s="2"/>
       <c r="F68" s="2"/>
-      <c r="G68" s="4" t="s">
+      <c r="G68" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="H68" s="4" t="s">
+      <c r="H68" s="5" t="s">
         <v>92</v>
       </c>
       <c r="I68" s="2">
@@ -4263,7 +4266,7 @@
       <c r="P68" s="2">
         <v>75</v>
       </c>
-      <c r="Q68" s="10"/>
+      <c r="Q68" s="11"/>
     </row>
     <row r="69" ht="17.6" spans="1:17">
       <c r="A69" s="2" t="s">
@@ -4280,10 +4283,10 @@
       </c>
       <c r="E69" s="2"/>
       <c r="F69" s="2"/>
-      <c r="G69" s="4" t="s">
+      <c r="G69" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="H69" s="4" t="s">
+      <c r="H69" s="5" t="s">
         <v>93</v>
       </c>
       <c r="I69" s="2">
@@ -4302,7 +4305,7 @@
       <c r="P69" s="2">
         <v>75</v>
       </c>
-      <c r="Q69" s="10"/>
+      <c r="Q69" s="11"/>
     </row>
     <row r="70" ht="17.6" spans="1:17">
       <c r="A70" s="2" t="s">
@@ -4319,10 +4322,10 @@
       </c>
       <c r="E70" s="2"/>
       <c r="F70" s="2"/>
-      <c r="G70" s="4" t="s">
+      <c r="G70" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="H70" s="4" t="s">
+      <c r="H70" s="5" t="s">
         <v>94</v>
       </c>
       <c r="I70" s="2">
@@ -4341,7 +4344,7 @@
       <c r="P70" s="2">
         <v>75</v>
       </c>
-      <c r="Q70" s="10"/>
+      <c r="Q70" s="11"/>
     </row>
     <row r="71" ht="17.6" spans="1:17">
       <c r="A71" s="2" t="s">
@@ -4358,10 +4361,10 @@
       </c>
       <c r="E71" s="2"/>
       <c r="F71" s="2"/>
-      <c r="G71" s="4" t="s">
+      <c r="G71" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="H71" s="4" t="s">
+      <c r="H71" s="5" t="s">
         <v>95</v>
       </c>
       <c r="I71" s="2">
@@ -4380,7 +4383,7 @@
       <c r="P71" s="2">
         <v>75</v>
       </c>
-      <c r="Q71" s="10"/>
+      <c r="Q71" s="11"/>
     </row>
     <row r="72" ht="17.6" spans="1:17">
       <c r="A72" s="2" t="s">
@@ -4397,10 +4400,10 @@
       </c>
       <c r="E72" s="2"/>
       <c r="F72" s="2"/>
-      <c r="G72" s="4" t="s">
+      <c r="G72" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="H72" s="4" t="s">
+      <c r="H72" s="5" t="s">
         <v>96</v>
       </c>
       <c r="I72" s="2">
@@ -4419,7 +4422,7 @@
       <c r="P72" s="2">
         <v>75</v>
       </c>
-      <c r="Q72" s="10"/>
+      <c r="Q72" s="11"/>
     </row>
     <row r="73" ht="17.6" spans="1:17">
       <c r="A73" s="2" t="s">
@@ -4436,10 +4439,10 @@
       </c>
       <c r="E73" s="2"/>
       <c r="F73" s="2"/>
-      <c r="G73" s="4" t="s">
+      <c r="G73" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="H73" s="4" t="s">
+      <c r="H73" s="5" t="s">
         <v>97</v>
       </c>
       <c r="I73" s="2">
@@ -4458,7 +4461,7 @@
       <c r="P73" s="2">
         <v>75</v>
       </c>
-      <c r="Q73" s="10"/>
+      <c r="Q73" s="11"/>
     </row>
     <row r="74" ht="17.6" spans="1:17">
       <c r="A74" s="2" t="s">
@@ -4475,10 +4478,10 @@
       </c>
       <c r="E74" s="2"/>
       <c r="F74" s="2"/>
-      <c r="G74" s="4" t="s">
+      <c r="G74" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="H74" s="4" t="s">
+      <c r="H74" s="5" t="s">
         <v>98</v>
       </c>
       <c r="I74" s="2">
@@ -4497,7 +4500,7 @@
       <c r="P74" s="2">
         <v>75</v>
       </c>
-      <c r="Q74" s="10"/>
+      <c r="Q74" s="11"/>
     </row>
     <row r="75" ht="17.6" spans="1:17">
       <c r="A75" s="2" t="s">
@@ -4514,10 +4517,10 @@
       </c>
       <c r="E75" s="2"/>
       <c r="F75" s="2"/>
-      <c r="G75" s="4" t="s">
+      <c r="G75" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="H75" s="4" t="s">
+      <c r="H75" s="5" t="s">
         <v>99</v>
       </c>
       <c r="I75" s="2">
@@ -4536,7 +4539,7 @@
       <c r="P75" s="2">
         <v>75</v>
       </c>
-      <c r="Q75" s="10"/>
+      <c r="Q75" s="11"/>
     </row>
     <row r="76" ht="17.6" spans="1:17">
       <c r="A76" s="2" t="s">
@@ -4553,10 +4556,10 @@
       </c>
       <c r="E76" s="2"/>
       <c r="F76" s="2"/>
-      <c r="G76" s="4" t="s">
+      <c r="G76" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="H76" s="4" t="s">
+      <c r="H76" s="5" t="s">
         <v>100</v>
       </c>
       <c r="I76" s="2">
@@ -4575,7 +4578,7 @@
       <c r="P76" s="2">
         <v>75</v>
       </c>
-      <c r="Q76" s="10"/>
+      <c r="Q76" s="11"/>
     </row>
     <row r="77" ht="17.6" spans="1:17">
       <c r="A77" s="2" t="s">
@@ -4592,10 +4595,10 @@
       </c>
       <c r="E77" s="2"/>
       <c r="F77" s="2"/>
-      <c r="G77" s="4" t="s">
+      <c r="G77" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="H77" s="4" t="s">
+      <c r="H77" s="5" t="s">
         <v>101</v>
       </c>
       <c r="I77" s="2">
@@ -4614,7 +4617,7 @@
       <c r="P77" s="2">
         <v>75</v>
       </c>
-      <c r="Q77" s="10"/>
+      <c r="Q77" s="11"/>
     </row>
     <row r="78" ht="17.6" spans="1:17">
       <c r="A78" s="2" t="s">
@@ -4631,10 +4634,10 @@
       </c>
       <c r="E78" s="2"/>
       <c r="F78" s="2"/>
-      <c r="G78" s="4" t="s">
+      <c r="G78" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="H78" s="4" t="s">
+      <c r="H78" s="5" t="s">
         <v>102</v>
       </c>
       <c r="I78" s="2">
@@ -4653,7 +4656,7 @@
       <c r="P78" s="2">
         <v>75</v>
       </c>
-      <c r="Q78" s="10"/>
+      <c r="Q78" s="11"/>
     </row>
     <row r="79" ht="17.6" spans="1:17">
       <c r="A79" s="2" t="s">
@@ -4670,10 +4673,10 @@
       </c>
       <c r="E79" s="2"/>
       <c r="F79" s="2"/>
-      <c r="G79" s="4" t="s">
+      <c r="G79" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="H79" s="4" t="s">
+      <c r="H79" s="5" t="s">
         <v>103</v>
       </c>
       <c r="I79" s="2">
@@ -4692,7 +4695,7 @@
       <c r="P79" s="2">
         <v>75</v>
       </c>
-      <c r="Q79" s="10"/>
+      <c r="Q79" s="11"/>
     </row>
     <row r="80" ht="17.6" spans="1:17">
       <c r="A80" s="2" t="s">
@@ -4709,10 +4712,10 @@
       </c>
       <c r="E80" s="2"/>
       <c r="F80" s="2"/>
-      <c r="G80" s="4" t="s">
+      <c r="G80" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="H80" s="4" t="s">
+      <c r="H80" s="5" t="s">
         <v>104</v>
       </c>
       <c r="I80" s="2">
@@ -4731,7 +4734,7 @@
       <c r="P80" s="2">
         <v>75</v>
       </c>
-      <c r="Q80" s="10"/>
+      <c r="Q80" s="11"/>
     </row>
     <row r="81" ht="17.6" spans="1:17">
       <c r="A81" s="2" t="s">
@@ -4748,10 +4751,10 @@
       </c>
       <c r="E81" s="2"/>
       <c r="F81" s="2"/>
-      <c r="G81" s="4" t="s">
+      <c r="G81" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="H81" s="4" t="s">
+      <c r="H81" s="5" t="s">
         <v>105</v>
       </c>
       <c r="I81" s="2">
@@ -4770,7 +4773,7 @@
       <c r="P81" s="2">
         <v>75</v>
       </c>
-      <c r="Q81" s="10"/>
+      <c r="Q81" s="11"/>
     </row>
     <row r="82" ht="17.6" spans="1:17">
       <c r="A82" s="2" t="s">
@@ -4787,10 +4790,10 @@
       </c>
       <c r="E82" s="2"/>
       <c r="F82" s="2"/>
-      <c r="G82" s="4" t="s">
+      <c r="G82" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="H82" s="4" t="s">
+      <c r="H82" s="5" t="s">
         <v>106</v>
       </c>
       <c r="I82" s="2">
@@ -4809,7 +4812,7 @@
       <c r="P82" s="2">
         <v>75</v>
       </c>
-      <c r="Q82" s="10"/>
+      <c r="Q82" s="11"/>
     </row>
     <row r="83" ht="17.6" spans="1:17">
       <c r="A83" s="2" t="s">
@@ -4826,27 +4829,27 @@
       </c>
       <c r="E83" s="2"/>
       <c r="F83" s="2"/>
-      <c r="G83" s="4" t="s">
+      <c r="G83" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="H83" s="4" t="s">
+      <c r="H83" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="I83" s="9">
+      <c r="I83" s="10">
         <v>2</v>
       </c>
-      <c r="J83" s="9"/>
+      <c r="J83" s="10"/>
       <c r="K83" s="2">
         <v>50</v>
       </c>
       <c r="L83" s="2"/>
       <c r="M83" s="2"/>
       <c r="N83" s="2"/>
-      <c r="O83" s="10"/>
+      <c r="O83" s="11"/>
       <c r="P83" s="2">
         <v>50</v>
       </c>
-      <c r="Q83" s="10"/>
+      <c r="Q83" s="11"/>
     </row>
     <row r="84" ht="17.6" spans="1:17">
       <c r="A84" s="2" t="s">
@@ -4863,27 +4866,27 @@
       </c>
       <c r="E84" s="2"/>
       <c r="F84" s="2"/>
-      <c r="G84" s="4" t="s">
+      <c r="G84" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="H84" s="4" t="s">
+      <c r="H84" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="I84" s="9">
+      <c r="I84" s="10">
         <v>2</v>
       </c>
-      <c r="J84" s="9"/>
+      <c r="J84" s="10"/>
       <c r="K84" s="2">
         <v>50</v>
       </c>
       <c r="L84" s="2"/>
       <c r="M84" s="2"/>
       <c r="N84" s="2"/>
-      <c r="O84" s="10"/>
+      <c r="O84" s="11"/>
       <c r="P84" s="2">
         <v>50</v>
       </c>
-      <c r="Q84" s="10"/>
+      <c r="Q84" s="11"/>
     </row>
     <row r="85" ht="17.6" spans="1:17">
       <c r="A85" s="2" t="s">
@@ -4900,27 +4903,27 @@
       </c>
       <c r="E85" s="2"/>
       <c r="F85" s="2"/>
-      <c r="G85" s="4" t="s">
+      <c r="G85" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="H85" s="4" t="s">
+      <c r="H85" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="I85" s="9">
+      <c r="I85" s="10">
         <v>2</v>
       </c>
-      <c r="J85" s="9"/>
+      <c r="J85" s="10"/>
       <c r="K85" s="2">
         <v>50</v>
       </c>
       <c r="L85" s="2"/>
       <c r="M85" s="2"/>
       <c r="N85" s="2"/>
-      <c r="O85" s="10"/>
+      <c r="O85" s="11"/>
       <c r="P85" s="2">
         <v>50</v>
       </c>
-      <c r="Q85" s="10"/>
+      <c r="Q85" s="11"/>
     </row>
     <row r="86" spans="1:17">
       <c r="A86" s="2" t="s">
@@ -4937,10 +4940,10 @@
       </c>
       <c r="E86" s="2"/>
       <c r="F86" s="2"/>
-      <c r="G86" s="4" t="s">
+      <c r="G86" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="H86" s="4" t="s">
+      <c r="H86" s="5" t="s">
         <v>111</v>
       </c>
       <c r="I86" s="2">

</xml_diff>